<commit_message>
edit survey covariates file
</commit_message>
<xml_diff>
--- a/code/istart_covariates_7june2022_simplified.xlsx
+++ b/code/istart_covariates_7june2022_simplified.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameswyngaarden/Documents/GitHub/istart-socdoors/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE72233-5A13-AC43-B8BB-36C97BD041D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D42A7CA-6CC3-C440-92A5-98E1ED679066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" tabRatio="985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11000" yWindow="500" windowWidth="17800" windowHeight="16460" tabRatio="985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="25">
   <si>
     <t>Sub</t>
   </si>
@@ -82,9 +82,6 @@
     <t>act_pcg</t>
   </si>
   <si>
-    <t>act_midbrain</t>
-  </si>
-  <si>
     <t>act_sma</t>
   </si>
   <si>
@@ -107,6 +104,12 @@
   </si>
   <si>
     <t>med RS</t>
+  </si>
+  <si>
+    <t>act_</t>
+  </si>
+  <si>
+    <t>act_frontal_operculum</t>
   </si>
 </sst>
 </file>
@@ -603,22 +606,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMI47"/>
+  <dimension ref="A1:AMJ47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AN29" sqref="AN29"/>
+    <sheetView tabSelected="1" topLeftCell="J17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="R47" sqref="R47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="1"/>
-    <col min="2" max="14" width="11.33203125" style="1"/>
-    <col min="15" max="16" width="14.33203125"/>
-    <col min="17" max="988" width="11.33203125" style="1"/>
-    <col min="989" max="1024" width="11.33203125"/>
+    <col min="2" max="12" width="11.33203125" style="1"/>
+    <col min="13" max="13" width="8.83203125" style="1"/>
+    <col min="14" max="15" width="11.33203125" style="1"/>
+    <col min="16" max="17" width="14.33203125"/>
+    <col min="18" max="989" width="11.33203125" style="1"/>
+    <col min="990" max="1025" width="11.33203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -656,33 +661,35 @@
         <v>11</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="N1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="P1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="Q1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="R1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="S1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="T1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="U1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="V1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="ALA1"/>
       <c r="ALB1"/>
       <c r="ALC1"/>
       <c r="ALD1"/>
@@ -717,8 +724,9 @@
       <c r="AMG1"/>
       <c r="AMH1"/>
       <c r="AMI1"/>
+      <c r="AMJ1"/>
     </row>
-    <row r="2" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1012</v>
       </c>
@@ -755,34 +763,34 @@
       <c r="L2" s="5">
         <v>-14.7036848654447</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="1"/>
+      <c r="N2">
         <v>-43.744684210000003</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>-26.558648340000001</v>
       </c>
-      <c r="O2" s="9">
+      <c r="P2" s="9">
         <v>22.838487700000002</v>
       </c>
-      <c r="P2" s="9">
+      <c r="Q2" s="9">
         <v>54.789193599999997</v>
       </c>
-      <c r="Q2" s="9">
+      <c r="R2" s="9">
         <v>-89.444519</v>
       </c>
-      <c r="R2" s="9">
+      <c r="S2" s="9">
         <v>-65.339265999999995</v>
       </c>
-      <c r="S2" s="10">
+      <c r="T2" s="10">
         <v>6.3950891500000004</v>
       </c>
-      <c r="T2" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="U2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="ALA2"/>
+        <v>20</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="ALB2"/>
       <c r="ALC2"/>
       <c r="ALD2"/>
@@ -817,8 +825,9 @@
       <c r="AMG2"/>
       <c r="AMH2"/>
       <c r="AMI2"/>
+      <c r="AMJ2"/>
     </row>
-    <row r="3" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1251</v>
       </c>
@@ -855,34 +864,34 @@
       <c r="L3" s="5">
         <v>-7.5071547596284498</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="1"/>
+      <c r="N3">
         <v>14.809717089999999</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>-27.583543110000001</v>
       </c>
-      <c r="O3" s="9">
+      <c r="P3" s="9">
         <v>28.457619699999999</v>
       </c>
-      <c r="P3" s="9">
+      <c r="Q3" s="9">
         <v>26.5186359</v>
       </c>
-      <c r="Q3" s="9">
+      <c r="R3" s="9">
         <v>-76.384567000000004</v>
       </c>
-      <c r="R3" s="9">
+      <c r="S3" s="9">
         <v>-151.88901999999999</v>
       </c>
-      <c r="S3" s="10">
+      <c r="T3" s="10">
         <v>17.331996700000001</v>
       </c>
-      <c r="T3" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="U3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="ALA3"/>
+        <v>20</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="ALB3"/>
       <c r="ALC3"/>
       <c r="ALD3"/>
@@ -917,8 +926,9 @@
       <c r="AMG3"/>
       <c r="AMH3"/>
       <c r="AMI3"/>
+      <c r="AMJ3"/>
     </row>
-    <row r="4" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3170</v>
       </c>
@@ -955,34 +965,34 @@
       <c r="L4" s="5">
         <v>-14.7036848654447</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="1"/>
+      <c r="N4">
         <v>7.2056715640000002</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>7.9489186719999996</v>
       </c>
-      <c r="O4" s="9">
+      <c r="P4" s="9">
         <v>45.655256100000003</v>
       </c>
-      <c r="P4" s="9">
+      <c r="Q4" s="9">
         <v>27.659606799999999</v>
       </c>
-      <c r="Q4" s="9">
+      <c r="R4" s="9">
         <v>-84.256866000000002</v>
       </c>
-      <c r="R4" s="9">
+      <c r="S4" s="9">
         <v>11.3170397</v>
       </c>
-      <c r="S4" s="10">
+      <c r="T4" s="10">
         <v>7.12791145</v>
       </c>
-      <c r="T4" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="U4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="ALA4"/>
+        <v>20</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="ALB4"/>
       <c r="ALC4"/>
       <c r="ALD4"/>
@@ -1017,8 +1027,9 @@
       <c r="AMG4"/>
       <c r="AMH4"/>
       <c r="AMI4"/>
+      <c r="AMJ4"/>
     </row>
-    <row r="5" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>3175</v>
       </c>
@@ -1055,34 +1066,34 @@
       <c r="L5" s="5">
         <v>-14.7036848654447</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="1"/>
+      <c r="N5">
         <v>82.179938070000006</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>-52.420184069999998</v>
       </c>
-      <c r="O5" s="9">
+      <c r="P5" s="9">
         <v>7.30699247</v>
       </c>
-      <c r="P5" s="9">
+      <c r="Q5" s="9">
         <v>144.81516099999999</v>
       </c>
-      <c r="Q5" s="9">
+      <c r="R5" s="9">
         <v>-128.07988</v>
       </c>
-      <c r="R5" s="9">
+      <c r="S5" s="9">
         <v>-358.61630000000002</v>
       </c>
-      <c r="S5" s="10">
+      <c r="T5" s="10">
         <v>8.4916185100000003</v>
       </c>
-      <c r="T5" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="U5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="ALA5"/>
+        <v>20</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="ALB5"/>
       <c r="ALC5"/>
       <c r="ALD5"/>
@@ -1117,8 +1128,9 @@
       <c r="AMG5"/>
       <c r="AMH5"/>
       <c r="AMI5"/>
+      <c r="AMJ5"/>
     </row>
-    <row r="6" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>1015</v>
       </c>
@@ -1155,34 +1167,34 @@
       <c r="L6" s="5">
         <v>13.2080581541674</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="1"/>
+      <c r="N6">
         <v>137.5536429</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>-37.040660770000002</v>
       </c>
-      <c r="O6" s="9">
+      <c r="P6" s="9">
         <v>9.8110612899999996</v>
       </c>
-      <c r="P6" s="9">
+      <c r="Q6" s="9">
         <v>8.7763971200000004</v>
       </c>
-      <c r="Q6" s="9">
+      <c r="R6" s="9">
         <v>-3.2836219999999998</v>
       </c>
-      <c r="R6" s="9">
+      <c r="S6" s="9">
         <v>-78.666763000000003</v>
       </c>
-      <c r="S6" s="10">
+      <c r="T6" s="10">
         <v>6.2024719700000004</v>
       </c>
-      <c r="T6" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="U6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="ALA6"/>
+        <v>20</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="ALB6"/>
       <c r="ALC6"/>
       <c r="ALD6"/>
@@ -1217,8 +1229,9 @@
       <c r="AMG6"/>
       <c r="AMH6"/>
       <c r="AMI6"/>
+      <c r="AMJ6"/>
     </row>
-    <row r="7" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>3166</v>
       </c>
@@ -1255,34 +1268,34 @@
       <c r="L7" s="5">
         <v>1.2364092629674399</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="1"/>
+      <c r="N7">
         <v>-10.141561340000001</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>-6.0681958199999997</v>
       </c>
-      <c r="O7" s="9">
+      <c r="P7" s="9">
         <v>69.3166899</v>
       </c>
-      <c r="P7" s="9">
+      <c r="Q7" s="9">
         <v>1.1984495100000001</v>
       </c>
-      <c r="Q7" s="9">
+      <c r="R7" s="9">
         <v>-44.105659000000003</v>
       </c>
-      <c r="R7" s="9">
+      <c r="S7" s="9">
         <v>-82.397115999999997</v>
       </c>
-      <c r="S7" s="10">
+      <c r="T7" s="10">
         <v>-20.147648799999999</v>
       </c>
-      <c r="T7" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="U7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="ALA7"/>
+        <v>20</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="ALB7"/>
       <c r="ALC7"/>
       <c r="ALD7"/>
@@ -1317,8 +1330,9 @@
       <c r="AMG7"/>
       <c r="AMH7"/>
       <c r="AMI7"/>
+      <c r="AMJ7"/>
     </row>
-    <row r="8" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>3176</v>
       </c>
@@ -1355,34 +1369,34 @@
       <c r="L8" s="5">
         <v>5.9507751350351201</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="1"/>
+      <c r="N8">
         <v>47.39930528</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>-7.1413466720000001</v>
       </c>
-      <c r="O8" s="9">
+      <c r="P8" s="9">
         <v>6.3353449199999998</v>
       </c>
-      <c r="P8" s="9">
+      <c r="Q8" s="9">
         <v>97.178318599999997</v>
       </c>
-      <c r="Q8" s="9">
+      <c r="R8" s="9">
         <v>44.9247704</v>
       </c>
-      <c r="R8" s="9">
+      <c r="S8" s="9">
         <v>-6.6006711999999998</v>
       </c>
-      <c r="S8" s="10">
+      <c r="T8" s="10">
         <v>1.61933613</v>
       </c>
-      <c r="T8" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="U8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="ALA8"/>
+        <v>20</v>
+      </c>
+      <c r="V8" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="ALB8"/>
       <c r="ALC8"/>
       <c r="ALD8"/>
@@ -1417,8 +1431,9 @@
       <c r="AMG8"/>
       <c r="AMH8"/>
       <c r="AMI8"/>
+      <c r="AMJ8"/>
     </row>
-    <row r="9" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>3200</v>
       </c>
@@ -1455,34 +1470,34 @@
       <c r="L9" s="5">
         <v>-3.1569388022654601</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="1"/>
+      <c r="N9">
         <v>-39.167937070000001</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>-10.59996668</v>
       </c>
-      <c r="O9" s="9">
+      <c r="P9" s="9">
         <v>-10.433695999999999</v>
       </c>
-      <c r="P9" s="9">
+      <c r="Q9" s="9">
         <v>134.91744399999999</v>
       </c>
-      <c r="Q9" s="9">
+      <c r="R9" s="9">
         <v>28.379520400000001</v>
       </c>
-      <c r="R9" s="9">
+      <c r="S9" s="9">
         <v>25.4298669</v>
       </c>
-      <c r="S9" s="10">
+      <c r="T9" s="10">
         <v>4.15968275</v>
       </c>
-      <c r="T9" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="U9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="ALA9"/>
+        <v>20</v>
+      </c>
+      <c r="V9" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="ALB9"/>
       <c r="ALC9"/>
       <c r="ALD9"/>
@@ -1517,8 +1532,9 @@
       <c r="AMG9"/>
       <c r="AMH9"/>
       <c r="AMI9"/>
+      <c r="AMJ9"/>
     </row>
-    <row r="10" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>3212</v>
       </c>
@@ -1555,34 +1571,34 @@
       <c r="L10" s="5">
         <v>-3.1569388022654601</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="1"/>
+      <c r="N10">
         <v>-42.168360450000002</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>-42.49175529</v>
       </c>
-      <c r="O10" s="9">
+      <c r="P10" s="9">
         <v>13.6012694</v>
       </c>
-      <c r="P10" s="9">
+      <c r="Q10" s="9">
         <v>70.448237700000007</v>
       </c>
-      <c r="Q10" s="9">
+      <c r="R10" s="9">
         <v>-60.202933999999999</v>
       </c>
-      <c r="R10" s="9">
+      <c r="S10" s="9">
         <v>2.5042821599999998</v>
       </c>
-      <c r="S10" s="10">
+      <c r="T10" s="10">
         <v>5.350276</v>
       </c>
-      <c r="T10" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="U10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="ALA10"/>
+        <v>20</v>
+      </c>
+      <c r="V10" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="ALB10"/>
       <c r="ALC10"/>
       <c r="ALD10"/>
@@ -1617,8 +1633,9 @@
       <c r="AMG10"/>
       <c r="AMH10"/>
       <c r="AMI10"/>
+      <c r="AMJ10"/>
     </row>
-    <row r="11" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>1245</v>
       </c>
@@ -1655,34 +1672,34 @@
       <c r="L11" s="5">
         <v>2.7781505534056099</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="1"/>
+      <c r="N11">
         <v>15.33062898</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <v>-34.288015459999997</v>
       </c>
-      <c r="O11" s="9">
+      <c r="P11" s="9">
         <v>30.846215300000001</v>
       </c>
-      <c r="P11" s="9">
+      <c r="Q11" s="9">
         <v>19.662128599999999</v>
       </c>
-      <c r="Q11" s="9">
+      <c r="R11" s="9">
         <v>-37.565967999999998</v>
       </c>
-      <c r="R11" s="9">
+      <c r="S11" s="9">
         <v>-13.801031</v>
       </c>
-      <c r="S11" s="10">
+      <c r="T11" s="10">
         <v>-0.52523613000000002</v>
       </c>
-      <c r="T11" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="U11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="ALA11"/>
+        <v>20</v>
+      </c>
+      <c r="V11" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="ALB11"/>
       <c r="ALC11"/>
       <c r="ALD11"/>
@@ -1717,8 +1734,9 @@
       <c r="AMG11"/>
       <c r="AMH11"/>
       <c r="AMI11"/>
+      <c r="AMJ11"/>
     </row>
-    <row r="12" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>1276</v>
       </c>
@@ -1755,34 +1773,34 @@
       <c r="L12" s="5">
         <v>5.5341603850737302</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="1"/>
+      <c r="N12">
         <v>-18.511118809999999</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <v>-58.791950059999998</v>
       </c>
-      <c r="O12" s="9">
+      <c r="P12" s="9">
         <v>-94.775426999999993</v>
       </c>
-      <c r="P12" s="9">
+      <c r="Q12" s="9">
         <v>22.9194055</v>
       </c>
-      <c r="Q12" s="9">
+      <c r="R12" s="9">
         <v>-4.0706252999999997</v>
       </c>
-      <c r="R12" s="9">
+      <c r="S12" s="9">
         <v>9.0527590500000006</v>
       </c>
-      <c r="S12" s="10">
+      <c r="T12" s="10">
         <v>3.8040723399999998</v>
       </c>
-      <c r="T12" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="U12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="ALA12"/>
+        <v>20</v>
+      </c>
+      <c r="V12" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="ALB12"/>
       <c r="ALC12"/>
       <c r="ALD12"/>
@@ -1817,8 +1835,9 @@
       <c r="AMG12"/>
       <c r="AMH12"/>
       <c r="AMI12"/>
+      <c r="AMJ12"/>
     </row>
-    <row r="13" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>1294</v>
       </c>
@@ -1855,34 +1874,34 @@
       <c r="L13" s="5">
         <v>5.0321531938017499</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="1"/>
+      <c r="N13">
         <v>41.22765502</v>
       </c>
-      <c r="N13">
+      <c r="O13">
         <v>-43.504668459999998</v>
       </c>
-      <c r="O13" s="9">
+      <c r="P13" s="9">
         <v>-6.5267790000000003</v>
       </c>
-      <c r="P13" s="9">
+      <c r="Q13" s="9">
         <v>60.975080200000001</v>
       </c>
-      <c r="Q13" s="9">
+      <c r="R13" s="9">
         <v>-31.702311000000002</v>
       </c>
-      <c r="R13" s="9">
+      <c r="S13" s="9">
         <v>-14.529658</v>
       </c>
-      <c r="S13" s="10">
+      <c r="T13" s="10">
         <v>6.85294282</v>
       </c>
-      <c r="T13" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="U13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="ALA13"/>
+        <v>20</v>
+      </c>
+      <c r="V13" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="ALB13"/>
       <c r="ALC13"/>
       <c r="ALD13"/>
@@ -1917,8 +1936,9 @@
       <c r="AMG13"/>
       <c r="AMH13"/>
       <c r="AMI13"/>
+      <c r="AMJ13"/>
     </row>
-    <row r="14" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>1301</v>
       </c>
@@ -1955,34 +1975,34 @@
       <c r="L14" s="5">
         <v>3.0241244287138098</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="1"/>
+      <c r="N14">
         <v>20.289118040000002</v>
       </c>
-      <c r="N14">
+      <c r="O14">
         <v>-52.688322890000002</v>
       </c>
-      <c r="O14" s="9">
+      <c r="P14" s="9">
         <v>-39.719687999999998</v>
       </c>
-      <c r="P14" s="9">
+      <c r="Q14" s="9">
         <v>85.316176999999996</v>
       </c>
-      <c r="Q14" s="9">
+      <c r="R14" s="9">
         <v>44.038662000000002</v>
       </c>
-      <c r="R14" s="9">
+      <c r="S14" s="9">
         <v>131.42799500000001</v>
       </c>
-      <c r="S14" s="10">
+      <c r="T14" s="10">
         <v>14.641844300000001</v>
       </c>
-      <c r="T14" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="U14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="ALA14"/>
+        <v>20</v>
+      </c>
+      <c r="V14" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="ALB14"/>
       <c r="ALC14"/>
       <c r="ALD14"/>
@@ -2017,8 +2037,9 @@
       <c r="AMG14"/>
       <c r="AMH14"/>
       <c r="AMI14"/>
+      <c r="AMJ14"/>
     </row>
-    <row r="15" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>3167</v>
       </c>
@@ -2055,34 +2076,34 @@
       <c r="L15" s="5">
         <v>5.0321531938017499</v>
       </c>
-      <c r="M15">
+      <c r="M15" s="1"/>
+      <c r="N15">
         <v>1.587598729</v>
       </c>
-      <c r="N15">
+      <c r="O15">
         <v>-2.7098392869999999</v>
       </c>
-      <c r="O15" s="9">
+      <c r="P15" s="9">
         <v>48.249327299999997</v>
       </c>
-      <c r="P15" s="9">
+      <c r="Q15" s="9">
         <v>50.172426799999997</v>
       </c>
-      <c r="Q15" s="9">
+      <c r="R15" s="9">
         <v>12.237022400000001</v>
       </c>
-      <c r="R15" s="9">
+      <c r="S15" s="9">
         <v>-58.242565999999997</v>
       </c>
-      <c r="S15" s="10">
+      <c r="T15" s="10">
         <v>6.7484929600000001</v>
       </c>
-      <c r="T15" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="U15" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="ALA15"/>
+        <v>20</v>
+      </c>
+      <c r="V15" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="ALB15"/>
       <c r="ALC15"/>
       <c r="ALD15"/>
@@ -2117,8 +2138,9 @@
       <c r="AMG15"/>
       <c r="AMH15"/>
       <c r="AMI15"/>
+      <c r="AMJ15"/>
     </row>
-    <row r="16" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>1010</v>
       </c>
@@ -2155,34 +2177,34 @@
       <c r="L16" s="5">
         <v>-17.229639436087101</v>
       </c>
-      <c r="M16">
+      <c r="M16" s="1"/>
+      <c r="N16">
         <v>136.85611660000001</v>
       </c>
-      <c r="N16">
+      <c r="O16">
         <v>1.2653025339999999</v>
       </c>
-      <c r="O16" s="9">
+      <c r="P16" s="9">
         <v>73.222070900000006</v>
       </c>
-      <c r="P16" s="9">
+      <c r="Q16" s="9">
         <v>61.411937299999998</v>
       </c>
-      <c r="Q16" s="9">
+      <c r="R16" s="9">
         <v>1.0866508500000001</v>
       </c>
-      <c r="R16" s="9">
+      <c r="S16" s="9">
         <v>60.556766600000003</v>
       </c>
-      <c r="S16" s="10">
+      <c r="T16" s="10">
         <v>-8.2675678099999992</v>
       </c>
-      <c r="T16" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="U16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="ALA16"/>
+        <v>20</v>
+      </c>
+      <c r="V16" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="ALB16"/>
       <c r="ALC16"/>
       <c r="ALD16"/>
@@ -2217,8 +2239,9 @@
       <c r="AMG16"/>
       <c r="AMH16"/>
       <c r="AMI16"/>
+      <c r="AMJ16"/>
     </row>
-    <row r="17" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>1021</v>
       </c>
@@ -2255,34 +2278,34 @@
       <c r="L17" s="5">
         <v>6.3167298563189496</v>
       </c>
-      <c r="M17">
+      <c r="M17" s="1"/>
+      <c r="N17">
         <v>24.766350419999998</v>
       </c>
-      <c r="N17">
+      <c r="O17">
         <v>-20.46612571</v>
       </c>
-      <c r="O17" s="9">
+      <c r="P17" s="9">
         <v>-51.911189</v>
       </c>
-      <c r="P17" s="9">
+      <c r="Q17" s="9">
         <v>68.3805835</v>
       </c>
-      <c r="Q17" s="9">
+      <c r="R17" s="9">
         <v>-15.590310000000001</v>
       </c>
-      <c r="R17" s="9">
+      <c r="S17" s="9">
         <v>-44.462949999999999</v>
       </c>
-      <c r="S17" s="10">
+      <c r="T17" s="10">
         <v>5.7089557700000002</v>
       </c>
-      <c r="T17" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="U17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="ALA17"/>
+        <v>20</v>
+      </c>
+      <c r="V17" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="ALB17"/>
       <c r="ALC17"/>
       <c r="ALD17"/>
@@ -2317,8 +2340,9 @@
       <c r="AMG17"/>
       <c r="AMH17"/>
       <c r="AMI17"/>
+      <c r="AMJ17"/>
     </row>
-    <row r="18" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>1243</v>
       </c>
@@ -2355,34 +2379,34 @@
       <c r="L18" s="5">
         <v>6.3167298563189496</v>
       </c>
-      <c r="M18">
+      <c r="M18" s="1"/>
+      <c r="N18">
         <v>-19.063366630000001</v>
       </c>
-      <c r="N18">
+      <c r="O18">
         <v>-11.88032216</v>
       </c>
-      <c r="O18" s="9">
+      <c r="P18" s="9">
         <v>-11.570719</v>
       </c>
-      <c r="P18" s="9">
+      <c r="Q18" s="9">
         <v>28.1792041</v>
       </c>
-      <c r="Q18" s="9">
+      <c r="R18" s="9">
         <v>68.790626500000002</v>
       </c>
-      <c r="R18" s="9">
+      <c r="S18" s="9">
         <v>55.120243299999998</v>
       </c>
-      <c r="S18" s="10">
+      <c r="T18" s="10">
         <v>5.8634147700000003</v>
       </c>
-      <c r="T18" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="U18" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="ALA18"/>
+        <v>20</v>
+      </c>
+      <c r="V18" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="ALB18"/>
       <c r="ALC18"/>
       <c r="ALD18"/>
@@ -2417,8 +2441,9 @@
       <c r="AMG18"/>
       <c r="AMH18"/>
       <c r="AMI18"/>
+      <c r="AMJ18"/>
     </row>
-    <row r="19" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>3140</v>
       </c>
@@ -2455,34 +2480,34 @@
       <c r="L19" s="5">
         <v>2.0124222509095899</v>
       </c>
-      <c r="M19">
+      <c r="M19" s="1"/>
+      <c r="N19">
         <v>41.97258978</v>
       </c>
-      <c r="N19">
+      <c r="O19">
         <v>-13.56885458</v>
       </c>
-      <c r="O19" s="9">
+      <c r="P19" s="9">
         <v>-41.793593000000001</v>
       </c>
-      <c r="P19" s="9">
+      <c r="Q19" s="9">
         <v>-7.4376822999999996</v>
       </c>
-      <c r="Q19" s="9">
+      <c r="R19" s="9">
         <v>44.8323441</v>
       </c>
-      <c r="R19" s="9">
+      <c r="S19" s="9">
         <v>10.9789168</v>
       </c>
-      <c r="S19" s="10">
+      <c r="T19" s="10">
         <v>-9.1280710700000007</v>
       </c>
-      <c r="T19" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="U19" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="ALA19"/>
+        <v>20</v>
+      </c>
+      <c r="V19" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="ALB19"/>
       <c r="ALC19"/>
       <c r="ALD19"/>
@@ -2517,8 +2542,9 @@
       <c r="AMG19"/>
       <c r="AMH19"/>
       <c r="AMI19"/>
+      <c r="AMJ19"/>
     </row>
-    <row r="20" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>1003</v>
       </c>
@@ -2555,34 +2581,34 @@
       <c r="L20" s="5">
         <v>2.9093413986700698</v>
       </c>
-      <c r="M20">
+      <c r="M20" s="1"/>
+      <c r="N20">
         <v>12.90129531</v>
       </c>
-      <c r="N20">
+      <c r="O20">
         <v>-15.89482918</v>
       </c>
-      <c r="O20" s="9">
+      <c r="P20" s="9">
         <v>113.864529</v>
       </c>
-      <c r="P20" s="9">
+      <c r="Q20" s="9">
         <v>-12.325996999999999</v>
       </c>
-      <c r="Q20" s="9">
+      <c r="R20" s="9">
         <v>24.9903297</v>
       </c>
-      <c r="R20" s="9">
+      <c r="S20" s="9">
         <v>61.768232400000002</v>
       </c>
-      <c r="S20" s="10">
+      <c r="T20" s="10">
         <v>-4.7663415699999998</v>
       </c>
-      <c r="T20" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="U20" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="ALA20"/>
+        <v>20</v>
+      </c>
+      <c r="V20" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="ALB20"/>
       <c r="ALC20"/>
       <c r="ALD20"/>
@@ -2617,8 +2643,9 @@
       <c r="AMG20"/>
       <c r="AMH20"/>
       <c r="AMI20"/>
+      <c r="AMJ20"/>
     </row>
-    <row r="21" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>1006</v>
       </c>
@@ -2655,34 +2682,34 @@
       <c r="L21" s="5">
         <v>12.0614027855197</v>
       </c>
-      <c r="M21">
+      <c r="M21" s="1"/>
+      <c r="N21">
         <v>21.993202879999998</v>
       </c>
-      <c r="N21">
+      <c r="O21">
         <v>-15.71320637</v>
       </c>
-      <c r="O21" s="9">
+      <c r="P21" s="9">
         <v>46.251495400000003</v>
       </c>
-      <c r="P21" s="9">
+      <c r="Q21" s="9">
         <v>36.107963400000003</v>
       </c>
-      <c r="Q21" s="9">
+      <c r="R21" s="9">
         <v>24.829212200000001</v>
       </c>
-      <c r="R21" s="9">
+      <c r="S21" s="9">
         <v>153.56662</v>
       </c>
-      <c r="S21" s="10">
+      <c r="T21" s="10">
         <v>-9.2136552300000005</v>
       </c>
-      <c r="T21" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="U21" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="ALA21"/>
+        <v>20</v>
+      </c>
+      <c r="V21" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="ALB21"/>
       <c r="ALC21"/>
       <c r="ALD21"/>
@@ -2717,8 +2744,9 @@
       <c r="AMG21"/>
       <c r="AMH21"/>
       <c r="AMI21"/>
+      <c r="AMJ21"/>
     </row>
-    <row r="22" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>1255</v>
       </c>
@@ -2755,34 +2783,34 @@
       <c r="L22" s="5">
         <v>0.621326051957662</v>
       </c>
-      <c r="M22">
+      <c r="M22" s="1"/>
+      <c r="N22">
         <v>34.020102899999998</v>
       </c>
-      <c r="N22">
+      <c r="O22">
         <v>48.960192599999999</v>
       </c>
-      <c r="O22" s="9">
+      <c r="P22" s="9">
         <v>-65.344363999999999</v>
       </c>
-      <c r="P22" s="9">
+      <c r="Q22" s="9">
         <v>12.029044600000001</v>
       </c>
-      <c r="Q22" s="9">
+      <c r="R22" s="9">
         <v>58.6439819</v>
       </c>
-      <c r="R22" s="9">
+      <c r="S22" s="9">
         <v>74.448393199999998</v>
       </c>
-      <c r="S22" s="10">
+      <c r="T22" s="10">
         <v>-1.89919949</v>
       </c>
-      <c r="T22" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="U22" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="ALA22"/>
+        <v>20</v>
+      </c>
+      <c r="V22" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="ALB22"/>
       <c r="ALC22"/>
       <c r="ALD22"/>
@@ -2817,8 +2845,9 @@
       <c r="AMG22"/>
       <c r="AMH22"/>
       <c r="AMI22"/>
+      <c r="AMJ22"/>
     </row>
-    <row r="23" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>3189</v>
       </c>
@@ -2855,34 +2884,34 @@
       <c r="L23" s="5">
         <v>0.12955666272931099</v>
       </c>
-      <c r="M23">
+      <c r="M23" s="1"/>
+      <c r="N23">
         <v>25.465853589999998</v>
       </c>
-      <c r="N23">
+      <c r="O23">
         <v>-42.647148860000001</v>
       </c>
-      <c r="O23" s="9">
+      <c r="P23" s="9">
         <v>40.314688599999997</v>
       </c>
-      <c r="P23" s="9">
+      <c r="Q23" s="9">
         <v>75.293011300000003</v>
       </c>
-      <c r="Q23" s="9">
+      <c r="R23" s="9">
         <v>52.198349</v>
       </c>
-      <c r="R23" s="9">
+      <c r="S23" s="9">
         <v>27.431182199999999</v>
       </c>
-      <c r="S23" s="10">
+      <c r="T23" s="10">
         <v>-21.740797499999999</v>
       </c>
-      <c r="T23" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="U23" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="ALA23"/>
+        <v>20</v>
+      </c>
+      <c r="V23" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="ALB23"/>
       <c r="ALC23"/>
       <c r="ALD23"/>
@@ -2917,8 +2946,9 @@
       <c r="AMG23"/>
       <c r="AMH23"/>
       <c r="AMI23"/>
+      <c r="AMJ23"/>
     </row>
-    <row r="24" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>3206</v>
       </c>
@@ -2955,34 +2985,34 @@
       <c r="L24" s="5">
         <v>-14.7196189625228</v>
       </c>
-      <c r="M24">
+      <c r="M24" s="1"/>
+      <c r="N24">
         <v>-17.74076835</v>
       </c>
-      <c r="N24">
+      <c r="O24">
         <v>50.625313949999999</v>
       </c>
-      <c r="O24" s="9">
+      <c r="P24" s="9">
         <v>18.8679378</v>
       </c>
-      <c r="P24" s="9">
+      <c r="Q24" s="9">
         <v>-34.455466999999999</v>
       </c>
-      <c r="Q24" s="9">
+      <c r="R24" s="9">
         <v>-5.7978095999999999</v>
       </c>
-      <c r="R24" s="9">
+      <c r="S24" s="9">
         <v>48.281009699999998</v>
       </c>
-      <c r="S24" s="10">
+      <c r="T24" s="10">
         <v>-26.221789399999999</v>
       </c>
-      <c r="T24" s="2" t="s">
+      <c r="U24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="V24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="U24" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="ALA24"/>
       <c r="ALB24"/>
       <c r="ALC24"/>
       <c r="ALD24"/>
@@ -3017,8 +3047,9 @@
       <c r="AMG24"/>
       <c r="AMH24"/>
       <c r="AMI24"/>
+      <c r="AMJ24"/>
     </row>
-    <row r="25" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>1001</v>
       </c>
@@ -3055,34 +3086,34 @@
       <c r="L25" s="5">
         <v>-0.94755924975467698</v>
       </c>
-      <c r="M25">
+      <c r="M25" s="1"/>
+      <c r="N25">
         <v>104.44815509999999</v>
       </c>
-      <c r="N25">
+      <c r="O25">
         <v>-39.978097750000003</v>
       </c>
-      <c r="O25" s="9">
+      <c r="P25" s="9">
         <v>38.503434400000003</v>
       </c>
-      <c r="P25" s="9">
+      <c r="Q25" s="9">
         <v>-13.475479999999999</v>
       </c>
-      <c r="Q25" s="9">
+      <c r="R25" s="9">
         <v>55.680831900000001</v>
       </c>
-      <c r="R25" s="9">
+      <c r="S25" s="9">
         <v>146.49041399999999</v>
       </c>
-      <c r="S25" s="10">
+      <c r="T25" s="10">
         <v>-4.8224854500000003</v>
       </c>
-      <c r="T25" s="2" t="s">
+      <c r="U25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="V25" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="U25" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="ALA25"/>
       <c r="ALB25"/>
       <c r="ALC25"/>
       <c r="ALD25"/>
@@ -3117,8 +3148,9 @@
       <c r="AMG25"/>
       <c r="AMH25"/>
       <c r="AMI25"/>
+      <c r="AMJ25"/>
     </row>
-    <row r="26" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>1286</v>
       </c>
@@ -3155,34 +3187,34 @@
       <c r="L26" s="5">
         <v>9.8472359097407605</v>
       </c>
-      <c r="M26">
+      <c r="M26" s="1"/>
+      <c r="N26">
         <v>30.1115259</v>
       </c>
-      <c r="N26">
+      <c r="O26">
         <v>49.45746879</v>
       </c>
-      <c r="O26" s="9">
+      <c r="P26" s="9">
         <v>4.3254374599999998</v>
       </c>
-      <c r="P26" s="9">
+      <c r="Q26" s="9">
         <v>-13.301997999999999</v>
       </c>
-      <c r="Q26" s="9">
+      <c r="R26" s="9">
         <v>-33.464962</v>
       </c>
-      <c r="R26" s="9">
+      <c r="S26" s="9">
         <v>28.920974099999999</v>
       </c>
-      <c r="S26" s="10">
+      <c r="T26" s="10">
         <v>-5.1670048199999998</v>
       </c>
-      <c r="T26" s="2" t="s">
+      <c r="U26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="V26" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="U26" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="ALA26"/>
       <c r="ALB26"/>
       <c r="ALC26"/>
       <c r="ALD26"/>
@@ -3217,8 +3249,9 @@
       <c r="AMG26"/>
       <c r="AMH26"/>
       <c r="AMI26"/>
+      <c r="AMJ26"/>
     </row>
-    <row r="27" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>1303</v>
       </c>
@@ -3255,34 +3288,34 @@
       <c r="L27" s="5">
         <v>-21.3110358858663</v>
       </c>
-      <c r="M27">
+      <c r="M27" s="1"/>
+      <c r="N27">
         <v>35.635082650000001</v>
       </c>
-      <c r="N27">
+      <c r="O27">
         <v>33.704344229999997</v>
       </c>
-      <c r="O27" s="9">
+      <c r="P27" s="9">
         <v>63.181349699999998</v>
       </c>
-      <c r="P27" s="9">
+      <c r="Q27" s="9">
         <v>-10.609337999999999</v>
       </c>
-      <c r="Q27" s="9">
+      <c r="R27" s="9">
         <v>51.451114699999998</v>
       </c>
-      <c r="R27" s="9">
+      <c r="S27" s="9">
         <v>54.760132499999997</v>
       </c>
-      <c r="S27" s="10">
+      <c r="T27" s="10">
         <v>16.345963999999999</v>
       </c>
-      <c r="T27" s="2" t="s">
+      <c r="U27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="V27" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="U27" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="ALA27"/>
       <c r="ALB27"/>
       <c r="ALC27"/>
       <c r="ALD27"/>
@@ -3317,8 +3350,9 @@
       <c r="AMG27"/>
       <c r="AMH27"/>
       <c r="AMI27"/>
+      <c r="AMJ27"/>
     </row>
-    <row r="28" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>3143</v>
       </c>
@@ -3355,34 +3389,34 @@
       <c r="L28" s="5">
         <v>-54.007188089647798</v>
       </c>
-      <c r="M28">
+      <c r="M28" s="1"/>
+      <c r="N28">
         <v>-2.0525630769999998</v>
       </c>
-      <c r="N28">
+      <c r="O28">
         <v>-17.27218384</v>
       </c>
-      <c r="O28" s="9">
+      <c r="P28" s="9">
         <v>-1.9140714000000001</v>
       </c>
-      <c r="P28" s="9">
+      <c r="Q28" s="9">
         <v>-13.370723999999999</v>
       </c>
-      <c r="Q28" s="9">
+      <c r="R28" s="9">
         <v>-16.247821999999999</v>
       </c>
-      <c r="R28" s="9">
+      <c r="S28" s="9">
         <v>-8.7662104000000003</v>
       </c>
-      <c r="S28" s="10">
+      <c r="T28" s="10">
         <v>-3.0872554800000001</v>
       </c>
-      <c r="T28" s="2" t="s">
+      <c r="U28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="V28" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="U28" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="ALA28"/>
       <c r="ALB28"/>
       <c r="ALC28"/>
       <c r="ALD28"/>
@@ -3417,8 +3451,9 @@
       <c r="AMG28"/>
       <c r="AMH28"/>
       <c r="AMI28"/>
+      <c r="AMJ28"/>
     </row>
-    <row r="29" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>1009</v>
       </c>
@@ -3455,34 +3490,34 @@
       <c r="L29" s="5">
         <v>9.9823289626171903</v>
       </c>
-      <c r="M29">
+      <c r="M29" s="1"/>
+      <c r="N29">
         <v>2.494506474</v>
       </c>
-      <c r="N29">
+      <c r="O29">
         <v>38.770238740000003</v>
       </c>
-      <c r="O29" s="9">
+      <c r="P29" s="9">
         <v>-6.4283463999999997</v>
       </c>
-      <c r="P29" s="9">
+      <c r="Q29" s="9">
         <v>-86.326468000000006</v>
       </c>
-      <c r="Q29" s="9">
+      <c r="R29" s="9">
         <v>20.4448471</v>
       </c>
-      <c r="R29" s="9">
+      <c r="S29" s="9">
         <v>20.850715000000001</v>
       </c>
-      <c r="S29" s="10">
+      <c r="T29" s="10">
         <v>16.786358799999999</v>
       </c>
-      <c r="T29" s="2" t="s">
+      <c r="U29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="V29" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="U29" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="ALA29"/>
       <c r="ALB29"/>
       <c r="ALC29"/>
       <c r="ALD29"/>
@@ -3517,8 +3552,9 @@
       <c r="AMG29"/>
       <c r="AMH29"/>
       <c r="AMI29"/>
+      <c r="AMJ29"/>
     </row>
-    <row r="30" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>1249</v>
       </c>
@@ -3555,34 +3591,34 @@
       <c r="L30" s="5">
         <v>2.5297985798186402</v>
       </c>
-      <c r="M30">
+      <c r="M30" s="1"/>
+      <c r="N30">
         <v>22.743217510000001</v>
       </c>
-      <c r="N30">
+      <c r="O30">
         <v>5.3051316379999998</v>
       </c>
-      <c r="O30" s="9">
+      <c r="P30" s="9">
         <v>-44.668028</v>
       </c>
-      <c r="P30" s="9">
+      <c r="Q30" s="9">
         <v>46.017015899999997</v>
       </c>
-      <c r="Q30" s="9">
+      <c r="R30" s="9">
         <v>-11.481002999999999</v>
       </c>
-      <c r="R30" s="9">
+      <c r="S30" s="9">
         <v>29.661425300000001</v>
       </c>
-      <c r="S30" s="10">
+      <c r="T30" s="10">
         <v>-9.6917865299999999</v>
       </c>
-      <c r="T30" s="2" t="s">
+      <c r="U30" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="V30" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="U30" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="ALA30"/>
       <c r="ALB30"/>
       <c r="ALC30"/>
       <c r="ALD30"/>
@@ -3617,8 +3653,9 @@
       <c r="AMG30"/>
       <c r="AMH30"/>
       <c r="AMI30"/>
+      <c r="AMJ30"/>
     </row>
-    <row r="31" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>3116</v>
       </c>
@@ -3655,34 +3692,34 @@
       <c r="L31" s="5">
         <v>8.2225695492040707</v>
       </c>
-      <c r="M31">
+      <c r="M31" s="1"/>
+      <c r="N31">
         <v>-10.87655007</v>
       </c>
-      <c r="N31">
+      <c r="O31">
         <v>-2.5690697899999999</v>
       </c>
-      <c r="O31" s="9">
+      <c r="P31" s="9">
         <v>46.590738000000002</v>
       </c>
-      <c r="P31" s="9">
+      <c r="Q31" s="9">
         <v>-93.432942999999995</v>
       </c>
-      <c r="Q31" s="9">
+      <c r="R31" s="9">
         <v>-26.289515000000002</v>
       </c>
-      <c r="R31" s="9">
+      <c r="S31" s="9">
         <v>-66.270713999999998</v>
       </c>
-      <c r="S31" s="10">
+      <c r="T31" s="10">
         <v>-21.8935125</v>
       </c>
-      <c r="T31" s="2" t="s">
+      <c r="U31" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="V31" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="U31" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="ALA31"/>
       <c r="ALB31"/>
       <c r="ALC31"/>
       <c r="ALD31"/>
@@ -3717,8 +3754,9 @@
       <c r="AMG31"/>
       <c r="AMH31"/>
       <c r="AMI31"/>
+      <c r="AMJ31"/>
     </row>
-    <row r="32" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>3199</v>
       </c>
@@ -3755,34 +3793,34 @@
       <c r="L32" s="5">
         <v>6.4628101357909404</v>
       </c>
-      <c r="M32">
+      <c r="M32" s="1"/>
+      <c r="N32">
         <v>38.044908</v>
       </c>
-      <c r="N32">
+      <c r="O32">
         <v>86.443887129999993</v>
       </c>
-      <c r="O32" s="9">
+      <c r="P32" s="9">
         <v>-82.625489000000002</v>
       </c>
-      <c r="P32" s="9">
+      <c r="Q32" s="9">
         <v>-6.5832949999999997</v>
       </c>
-      <c r="Q32" s="9">
+      <c r="R32" s="9">
         <v>108.666901</v>
       </c>
-      <c r="R32" s="9">
+      <c r="S32" s="9">
         <v>3.0840355599999998</v>
       </c>
-      <c r="S32" s="10">
+      <c r="T32" s="10">
         <v>-21.5328555</v>
       </c>
-      <c r="T32" s="2" t="s">
+      <c r="U32" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="V32" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="U32" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="ALA32"/>
       <c r="ALB32"/>
       <c r="ALC32"/>
       <c r="ALD32"/>
@@ -3817,8 +3855,9 @@
       <c r="AMG32"/>
       <c r="AMH32"/>
       <c r="AMI32"/>
+      <c r="AMJ32"/>
     </row>
-    <row r="33" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="11">
         <v>3220</v>
       </c>
@@ -3855,34 +3894,34 @@
       <c r="L33" s="5">
         <v>2.9432913089646902</v>
       </c>
-      <c r="M33">
+      <c r="M33" s="1"/>
+      <c r="N33">
         <v>6.1268146100000003</v>
       </c>
-      <c r="N33">
+      <c r="O33">
         <v>4.0158694229999998</v>
       </c>
-      <c r="O33" s="9">
+      <c r="P33" s="9">
         <v>36.241843699999997</v>
       </c>
-      <c r="P33" s="9">
+      <c r="Q33" s="9">
         <v>4.95889588</v>
       </c>
-      <c r="Q33" s="9">
+      <c r="R33" s="9">
         <v>-12.92651</v>
       </c>
-      <c r="R33" s="9">
+      <c r="S33" s="9">
         <v>77.791620899999998</v>
       </c>
-      <c r="S33" s="10">
+      <c r="T33" s="10">
         <v>1.3800907099999999</v>
       </c>
-      <c r="T33" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="U33" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="ALA33"/>
+        <v>21</v>
+      </c>
+      <c r="V33" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="ALB33"/>
       <c r="ALC33"/>
       <c r="ALD33"/>
@@ -3917,8 +3956,9 @@
       <c r="AMG33"/>
       <c r="AMH33"/>
       <c r="AMI33"/>
+      <c r="AMJ33"/>
     </row>
-    <row r="34" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>1004</v>
       </c>
@@ -3955,34 +3995,34 @@
       <c r="L34" s="5">
         <v>3.6438235302250002</v>
       </c>
-      <c r="M34">
+      <c r="M34" s="1"/>
+      <c r="N34">
         <v>-39.001481699999999</v>
       </c>
-      <c r="N34">
+      <c r="O34">
         <v>-0.43271195109999999</v>
       </c>
-      <c r="O34" s="9">
+      <c r="P34" s="9">
         <v>10.4736101</v>
       </c>
-      <c r="P34" s="9">
+      <c r="Q34" s="9">
         <v>-24.121327999999998</v>
       </c>
-      <c r="Q34" s="9">
+      <c r="R34" s="9">
         <v>32.432022099999998</v>
       </c>
-      <c r="R34" s="9">
+      <c r="S34" s="9">
         <v>-28.917687000000001</v>
       </c>
-      <c r="S34" s="10">
+      <c r="T34" s="10">
         <v>-7.2744746200000003</v>
       </c>
-      <c r="T34" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="U34" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="ALA34"/>
+        <v>21</v>
+      </c>
+      <c r="V34" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="ALB34"/>
       <c r="ALC34"/>
       <c r="ALD34"/>
@@ -4017,8 +4057,9 @@
       <c r="AMG34"/>
       <c r="AMH34"/>
       <c r="AMI34"/>
+      <c r="AMJ34"/>
     </row>
-    <row r="35" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>1019</v>
       </c>
@@ -4055,34 +4096,34 @@
       <c r="L35" s="5">
         <v>3.0160411167388999</v>
       </c>
-      <c r="M35">
+      <c r="M35" s="1"/>
+      <c r="N35">
         <v>-32.559631869999997</v>
       </c>
-      <c r="N35">
+      <c r="O35">
         <v>25.00740184</v>
       </c>
-      <c r="O35" s="9">
+      <c r="P35" s="9">
         <v>-20.744482999999999</v>
       </c>
-      <c r="P35" s="9">
+      <c r="Q35" s="9">
         <v>-42.182209999999998</v>
       </c>
-      <c r="Q35" s="9">
+      <c r="R35" s="9">
         <v>-34.189720000000001</v>
       </c>
-      <c r="R35" s="9">
+      <c r="S35" s="9">
         <v>54.625435400000001</v>
       </c>
-      <c r="S35" s="10">
+      <c r="T35" s="10">
         <v>-18.1640902</v>
       </c>
-      <c r="T35" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="U35" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="ALA35"/>
+        <v>21</v>
+      </c>
+      <c r="V35" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="ALB35"/>
       <c r="ALC35"/>
       <c r="ALD35"/>
@@ -4117,8 +4158,9 @@
       <c r="AMG35"/>
       <c r="AMH35"/>
       <c r="AMI35"/>
+      <c r="AMJ35"/>
     </row>
-    <row r="36" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>1242</v>
       </c>
@@ -4155,34 +4197,34 @@
       <c r="L36" s="5">
         <v>-0.122870950691603</v>
       </c>
-      <c r="M36">
+      <c r="M36" s="1"/>
+      <c r="N36">
         <v>-29.55395721</v>
       </c>
-      <c r="N36">
+      <c r="O36">
         <v>-15.142114680000001</v>
       </c>
-      <c r="O36" s="9">
+      <c r="P36" s="9">
         <v>-1.6757515000000001</v>
       </c>
-      <c r="P36" s="9">
+      <c r="Q36" s="9">
         <v>-52.677019000000001</v>
       </c>
-      <c r="Q36" s="9">
+      <c r="R36" s="9">
         <v>-54.459502999999998</v>
       </c>
-      <c r="R36" s="9">
+      <c r="S36" s="9">
         <v>12.1930508</v>
       </c>
-      <c r="S36" s="10">
+      <c r="T36" s="10">
         <v>-3.6567214699999999</v>
       </c>
-      <c r="T36" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="U36" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="ALA36"/>
+        <v>21</v>
+      </c>
+      <c r="V36" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="ALB36"/>
       <c r="ALC36"/>
       <c r="ALD36"/>
@@ -4217,8 +4259,9 @@
       <c r="AMG36"/>
       <c r="AMH36"/>
       <c r="AMI36"/>
+      <c r="AMJ36"/>
     </row>
-    <row r="37" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>1247</v>
       </c>
@@ -4255,34 +4298,34 @@
       <c r="L37" s="5">
         <v>4.2716059437110996</v>
       </c>
-      <c r="M37">
+      <c r="M37" s="1"/>
+      <c r="N37">
         <v>11.71056053</v>
       </c>
-      <c r="N37">
+      <c r="O37">
         <v>-9.2690660359999999</v>
       </c>
-      <c r="O37" s="9">
+      <c r="P37" s="9">
         <v>18.243709299999999</v>
       </c>
-      <c r="P37" s="9">
+      <c r="Q37" s="9">
         <v>-7.7070542</v>
       </c>
-      <c r="Q37" s="9">
+      <c r="R37" s="9">
         <v>-3.2709765000000002</v>
       </c>
-      <c r="R37" s="9">
+      <c r="S37" s="9">
         <v>-19.080860999999999</v>
       </c>
-      <c r="S37" s="10">
+      <c r="T37" s="10">
         <v>2.5315623299999999</v>
       </c>
-      <c r="T37" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="U37" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="ALA37"/>
+        <v>21</v>
+      </c>
+      <c r="V37" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="ALB37"/>
       <c r="ALC37"/>
       <c r="ALD37"/>
@@ -4317,8 +4360,9 @@
       <c r="AMG37"/>
       <c r="AMH37"/>
       <c r="AMI37"/>
+      <c r="AMJ37"/>
     </row>
-    <row r="38" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>1248</v>
       </c>
@@ -4355,34 +4399,34 @@
       <c r="L38" s="5">
         <v>6.1549531841693899</v>
       </c>
-      <c r="M38">
+      <c r="M38" s="1"/>
+      <c r="N38">
         <v>18.935483290000001</v>
       </c>
-      <c r="N38">
+      <c r="O38">
         <v>-24.186613879999999</v>
       </c>
-      <c r="O38" s="9">
+      <c r="P38" s="9">
         <v>20.920466900000001</v>
       </c>
-      <c r="P38" s="9">
+      <c r="Q38" s="9">
         <v>-19.400817</v>
       </c>
-      <c r="Q38" s="9">
+      <c r="R38" s="9">
         <v>6.9297866800000003</v>
       </c>
-      <c r="R38" s="9">
+      <c r="S38" s="9">
         <v>51.871139100000001</v>
       </c>
-      <c r="S38" s="10">
+      <c r="T38" s="10">
         <v>-4.78914654</v>
       </c>
-      <c r="T38" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="U38" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="ALA38"/>
+        <v>21</v>
+      </c>
+      <c r="V38" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="ALB38"/>
       <c r="ALC38"/>
       <c r="ALD38"/>
@@ -4417,8 +4461,9 @@
       <c r="AMG38"/>
       <c r="AMH38"/>
       <c r="AMI38"/>
+      <c r="AMJ38"/>
     </row>
-    <row r="39" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>1016</v>
       </c>
@@ -4455,34 +4500,34 @@
       <c r="L39" s="5">
         <v>-1.2050682749057</v>
       </c>
-      <c r="M39">
+      <c r="M39" s="1"/>
+      <c r="N39">
         <v>20.234945719999999</v>
       </c>
-      <c r="N39">
+      <c r="O39">
         <v>24.458773480000001</v>
       </c>
-      <c r="O39" s="9">
+      <c r="P39" s="9">
         <v>7.9480848799999997</v>
       </c>
-      <c r="P39" s="9">
+      <c r="Q39" s="9">
         <v>-6.1042287000000002</v>
       </c>
-      <c r="Q39" s="9">
+      <c r="R39" s="9">
         <v>55.617233300000002</v>
       </c>
-      <c r="R39" s="9">
+      <c r="S39" s="9">
         <v>-33.822575999999998</v>
       </c>
-      <c r="S39" s="10">
+      <c r="T39" s="10">
         <v>2.7318754200000002</v>
       </c>
-      <c r="T39" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="U39" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="ALA39"/>
+        <v>21</v>
+      </c>
+      <c r="V39" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="ALB39"/>
       <c r="ALC39"/>
       <c r="ALD39"/>
@@ -4517,8 +4562,9 @@
       <c r="AMG39"/>
       <c r="AMH39"/>
       <c r="AMI39"/>
+      <c r="AMJ39"/>
     </row>
-    <row r="40" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>3122</v>
       </c>
@@ -4555,34 +4601,34 @@
       <c r="L40" s="5">
         <v>-2.2878288835315401</v>
       </c>
-      <c r="M40">
+      <c r="M40" s="1"/>
+      <c r="N40">
         <v>31.814467520000001</v>
       </c>
-      <c r="N40">
+      <c r="O40">
         <v>16.516538329999999</v>
       </c>
-      <c r="O40" s="9">
+      <c r="P40" s="9">
         <v>19.466499299999999</v>
       </c>
-      <c r="P40" s="9">
+      <c r="Q40" s="9">
         <v>-19.626802000000001</v>
       </c>
-      <c r="Q40" s="9">
+      <c r="R40" s="9">
         <v>-85.757598999999999</v>
       </c>
-      <c r="R40" s="9">
+      <c r="S40" s="9">
         <v>101.186187</v>
       </c>
-      <c r="S40" s="10">
+      <c r="T40" s="10">
         <v>-7.6465631700000003</v>
       </c>
-      <c r="T40" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="U40" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="ALA40"/>
+        <v>21</v>
+      </c>
+      <c r="V40" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="ALB40"/>
       <c r="ALC40"/>
       <c r="ALD40"/>
@@ -4617,8 +4663,9 @@
       <c r="AMG40"/>
       <c r="AMH40"/>
       <c r="AMI40"/>
+      <c r="AMJ40"/>
     </row>
-    <row r="41" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>3173</v>
       </c>
@@ -4655,34 +4702,34 @@
       <c r="L41" s="5">
         <v>-1.2050682749057</v>
       </c>
-      <c r="M41">
+      <c r="M41" s="1"/>
+      <c r="N41">
         <v>-19.016999760000001</v>
       </c>
-      <c r="N41">
+      <c r="O41">
         <v>16.06320122</v>
       </c>
-      <c r="O41" s="9">
+      <c r="P41" s="9">
         <v>43.165981199999997</v>
       </c>
-      <c r="P41" s="9">
+      <c r="Q41" s="9">
         <v>5.2897953900000001</v>
       </c>
-      <c r="Q41" s="9">
+      <c r="R41" s="9">
         <v>31.54599</v>
       </c>
-      <c r="R41" s="9">
+      <c r="S41" s="9">
         <v>-38.129936000000001</v>
       </c>
-      <c r="S41" s="10">
+      <c r="T41" s="10">
         <v>14.1987691</v>
       </c>
-      <c r="T41" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="U41" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="ALA41"/>
+        <v>21</v>
+      </c>
+      <c r="V41" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="ALB41"/>
       <c r="ALC41"/>
       <c r="ALD41"/>
@@ -4717,8 +4764,9 @@
       <c r="AMG41"/>
       <c r="AMH41"/>
       <c r="AMI41"/>
+      <c r="AMJ41"/>
     </row>
-    <row r="42" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>3190</v>
       </c>
@@ -4755,34 +4803,34 @@
       <c r="L42" s="5">
         <v>1.2148704699125601</v>
       </c>
-      <c r="M42">
+      <c r="M42" s="1"/>
+      <c r="N42">
         <v>-13.36074223</v>
       </c>
-      <c r="N42">
+      <c r="O42">
         <v>13.81822288</v>
       </c>
-      <c r="O42" s="9">
+      <c r="P42" s="9">
         <v>2.8126172</v>
       </c>
-      <c r="P42" s="9">
+      <c r="Q42" s="9">
         <v>-42.151594000000003</v>
       </c>
-      <c r="Q42" s="9">
+      <c r="R42" s="9">
         <v>1.5118923200000001</v>
       </c>
-      <c r="R42" s="9">
+      <c r="S42" s="9">
         <v>-27.455165000000001</v>
       </c>
-      <c r="S42" s="10">
+      <c r="T42" s="10">
         <v>11.153667199999999</v>
       </c>
-      <c r="T42" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="U42" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="ALA42"/>
+        <v>21</v>
+      </c>
+      <c r="V42" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="ALB42"/>
       <c r="ALC42"/>
       <c r="ALD42"/>
@@ -4817,8 +4865,9 @@
       <c r="AMG42"/>
       <c r="AMH42"/>
       <c r="AMI42"/>
+      <c r="AMJ42"/>
     </row>
-    <row r="43" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>1013</v>
       </c>
@@ -4855,34 +4904,34 @@
       <c r="L43" s="5">
         <v>-6.0932141546602203</v>
       </c>
-      <c r="M43">
+      <c r="M43" s="1"/>
+      <c r="N43">
         <v>22.57061805</v>
       </c>
-      <c r="N43">
+      <c r="O43">
         <v>14.10674626</v>
       </c>
-      <c r="O43" s="9">
+      <c r="P43" s="9">
         <v>29.8245857</v>
       </c>
-      <c r="P43" s="9">
+      <c r="Q43" s="9">
         <v>-2.0499497999999998</v>
       </c>
-      <c r="Q43" s="9">
+      <c r="R43" s="9">
         <v>25.567386599999999</v>
       </c>
-      <c r="R43" s="9">
+      <c r="S43" s="9">
         <v>-35.967784999999999</v>
       </c>
-      <c r="S43" s="10">
+      <c r="T43" s="10">
         <v>26.907920399999998</v>
       </c>
-      <c r="T43" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="U43" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="ALA43"/>
+        <v>21</v>
+      </c>
+      <c r="V43" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="ALB43"/>
       <c r="ALC43"/>
       <c r="ALD43"/>
@@ -4917,8 +4966,9 @@
       <c r="AMG43"/>
       <c r="AMH43"/>
       <c r="AMI43"/>
+      <c r="AMJ43"/>
     </row>
-    <row r="44" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>1244</v>
       </c>
@@ -4955,34 +5005,34 @@
       <c r="L44" s="5">
         <v>22.576882184926401</v>
       </c>
-      <c r="M44">
+      <c r="M44" s="1"/>
+      <c r="N44">
         <v>-68.809409819999999</v>
       </c>
-      <c r="N44">
+      <c r="O44">
         <v>34.58474485</v>
       </c>
-      <c r="O44" s="9">
+      <c r="P44" s="9">
         <v>-13.414370999999999</v>
       </c>
-      <c r="P44" s="9">
+      <c r="Q44" s="9">
         <v>-67.723850999999996</v>
       </c>
-      <c r="Q44" s="9">
+      <c r="R44" s="9">
         <v>-25.997807000000002</v>
       </c>
-      <c r="R44" s="9">
+      <c r="S44" s="9">
         <v>13.7213434</v>
       </c>
-      <c r="S44" s="10">
+      <c r="T44" s="10">
         <v>18.834749200000001</v>
       </c>
-      <c r="T44" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="U44" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="ALA44"/>
+        <v>21</v>
+      </c>
+      <c r="V44" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="ALB44"/>
       <c r="ALC44"/>
       <c r="ALD44"/>
@@ -5017,8 +5067,9 @@
       <c r="AMG44"/>
       <c r="AMH44"/>
       <c r="AMI44"/>
+      <c r="AMJ44"/>
     </row>
-    <row r="45" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>1302</v>
       </c>
@@ -5055,34 +5106,34 @@
       <c r="L45" s="5">
         <v>16.693002043695699</v>
       </c>
-      <c r="M45">
+      <c r="M45" s="1"/>
+      <c r="N45">
         <v>-14.12548196</v>
       </c>
-      <c r="N45">
+      <c r="O45">
         <v>73.967896420000002</v>
       </c>
-      <c r="O45" s="9">
+      <c r="P45" s="9">
         <v>4.4540231300000004</v>
       </c>
-      <c r="P45" s="9">
+      <c r="Q45" s="9">
         <v>-13.722413</v>
       </c>
-      <c r="Q45" s="9">
+      <c r="R45" s="9">
         <v>-25.413962999999999</v>
       </c>
-      <c r="R45" s="9">
+      <c r="S45" s="9">
         <v>-119.47413</v>
       </c>
-      <c r="S45" s="10">
+      <c r="T45" s="10">
         <v>16.962341899999998</v>
       </c>
-      <c r="T45" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="U45" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="ALA45"/>
+        <v>21</v>
+      </c>
+      <c r="V45" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="ALB45"/>
       <c r="ALC45"/>
       <c r="ALD45"/>
@@ -5117,8 +5168,9 @@
       <c r="AMG45"/>
       <c r="AMH45"/>
       <c r="AMI45"/>
+      <c r="AMJ45"/>
     </row>
-    <row r="46" spans="1:1023" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>3125</v>
       </c>
@@ -5155,34 +5207,34 @@
       <c r="L46" s="5">
         <v>4.0653825966195898</v>
       </c>
-      <c r="M46">
+      <c r="M46" s="1"/>
+      <c r="N46">
         <v>-7.693539683</v>
       </c>
-      <c r="N46">
+      <c r="O46">
         <v>12.807463630000001</v>
       </c>
-      <c r="O46" s="9">
+      <c r="P46" s="9">
         <v>-3.6277621999999998</v>
       </c>
-      <c r="P46" s="9">
+      <c r="Q46" s="9">
         <v>-70.314953000000003</v>
       </c>
-      <c r="Q46" s="9">
+      <c r="R46" s="9">
         <v>-104.09634</v>
       </c>
-      <c r="R46" s="9">
+      <c r="S46" s="9">
         <v>-62.864939999999997</v>
       </c>
-      <c r="S46" s="10">
+      <c r="T46" s="10">
         <v>61.729894600000002</v>
       </c>
-      <c r="T46" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="U46" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="ALA46"/>
+        <v>21</v>
+      </c>
+      <c r="V46" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="ALB46"/>
       <c r="ALC46"/>
       <c r="ALD46"/>
@@ -5217,8 +5269,9 @@
       <c r="AMG46"/>
       <c r="AMH46"/>
       <c r="AMI46"/>
+      <c r="AMJ46"/>
     </row>
-    <row r="47" spans="1:1023" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1024" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="6">
         <v>3152</v>
       </c>
@@ -5255,34 +5308,34 @@
       <c r="L47" s="7">
         <v>3.2730904375410899</v>
       </c>
-      <c r="M47">
+      <c r="M47" s="1"/>
+      <c r="N47">
         <v>2.5933439730000001</v>
       </c>
-      <c r="N47">
+      <c r="O47">
         <v>-36.52316012</v>
       </c>
-      <c r="O47" s="9">
+      <c r="P47" s="9">
         <v>-84.384434999999996</v>
       </c>
-      <c r="P47" s="9">
+      <c r="Q47" s="9">
         <v>-117.61387000000001</v>
       </c>
-      <c r="Q47" s="9">
+      <c r="R47" s="9">
         <v>-415.90964000000002</v>
       </c>
-      <c r="R47" s="9">
+      <c r="S47" s="9">
         <v>-236.70777000000001</v>
       </c>
-      <c r="S47" s="10">
+      <c r="T47" s="10">
         <v>53.062666900000004</v>
       </c>
-      <c r="T47" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="U47" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="ALA47"/>
+        <v>21</v>
+      </c>
+      <c r="V47" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="ALB47"/>
       <c r="ALC47"/>
       <c r="ALD47"/>
@@ -5317,9 +5370,10 @@
       <c r="AMG47"/>
       <c r="AMH47"/>
       <c r="AMI47"/>
+      <c r="AMJ47"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U47">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:V47">
     <sortCondition ref="H1:H47"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
edit for residual testing
</commit_message>
<xml_diff>
--- a/code/istart_covariates_7june2022_simplified.xlsx
+++ b/code/istart_covariates_7june2022_simplified.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameswyngaarden/Documents/GitHub/istart-socdoors/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D42A7CA-6CC3-C440-92A5-98E1ED679066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB3D17AA-445B-764C-A2EF-E15CA994ECA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11000" yWindow="500" windowWidth="17800" windowHeight="16460" tabRatio="985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="16480" tabRatio="985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="27">
   <si>
     <t>Sub</t>
   </si>
@@ -110,6 +110,12 @@
   </si>
   <si>
     <t>act_frontal_operculum</t>
+  </si>
+  <si>
+    <t>fd_mean_cont</t>
+  </si>
+  <si>
+    <t>tsnr_cont</t>
   </si>
 </sst>
 </file>
@@ -606,24 +612,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMJ47"/>
+  <dimension ref="A1:AML47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="R47" sqref="R47"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47:G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="1"/>
-    <col min="2" max="12" width="11.33203125" style="1"/>
-    <col min="13" max="13" width="8.83203125" style="1"/>
-    <col min="14" max="15" width="11.33203125" style="1"/>
-    <col min="16" max="17" width="14.33203125"/>
-    <col min="18" max="989" width="11.33203125" style="1"/>
-    <col min="990" max="1025" width="11.33203125"/>
+    <col min="2" max="5" width="11.33203125" style="1"/>
+    <col min="6" max="7" width="8.83203125" style="1"/>
+    <col min="8" max="14" width="11.33203125" style="1"/>
+    <col min="15" max="15" width="8.83203125" style="1"/>
+    <col min="16" max="17" width="11.33203125" style="1"/>
+    <col min="18" max="19" width="14.33203125"/>
+    <col min="20" max="991" width="11.33203125" style="1"/>
+    <col min="992" max="1027" width="11.33203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -640,58 +648,62 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="P1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="Q1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="R1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="T1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="U1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="V1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="W1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="X1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="ALB1"/>
-      <c r="ALC1"/>
       <c r="ALD1"/>
       <c r="ALE1"/>
       <c r="ALF1"/>
@@ -725,8 +737,10 @@
       <c r="AMH1"/>
       <c r="AMI1"/>
       <c r="AMJ1"/>
+      <c r="AMK1"/>
+      <c r="AML1"/>
     </row>
-    <row r="2" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1012</v>
       </c>
@@ -743,56 +757,62 @@
         <v>0.48350004595225998</v>
       </c>
       <c r="F2" s="2">
+        <f>B2-D2</f>
+        <v>-4.8793055871598989E-2</v>
+      </c>
+      <c r="G2" s="2">
+        <f>C2-E2</f>
+        <v>1.00805258004631</v>
+      </c>
+      <c r="H2" s="2">
         <v>-0.60577960340705195</v>
       </c>
-      <c r="G2" s="2">
+      <c r="I2" s="2">
         <v>0.98752633597541495</v>
       </c>
-      <c r="H2" s="2">
+      <c r="J2" s="2">
         <v>-4.5434782608695699</v>
       </c>
-      <c r="I2" s="2">
+      <c r="K2" s="2">
         <v>12.438563327032099</v>
       </c>
-      <c r="J2" s="2">
+      <c r="L2" s="2">
         <v>-1.4278234379200101</v>
       </c>
-      <c r="K2" s="2">
+      <c r="M2" s="2">
         <v>5.9975282647079604</v>
       </c>
-      <c r="L2" s="5">
+      <c r="N2" s="5">
         <v>-14.7036848654447</v>
       </c>
-      <c r="M2" s="1"/>
-      <c r="N2">
+      <c r="O2" s="1"/>
+      <c r="P2">
         <v>-43.744684210000003</v>
       </c>
-      <c r="O2">
+      <c r="Q2">
         <v>-26.558648340000001</v>
       </c>
-      <c r="P2" s="9">
+      <c r="R2" s="9">
         <v>22.838487700000002</v>
       </c>
-      <c r="Q2" s="9">
+      <c r="S2" s="9">
         <v>54.789193599999997</v>
       </c>
-      <c r="R2" s="9">
+      <c r="T2" s="9">
         <v>-89.444519</v>
       </c>
-      <c r="S2" s="9">
+      <c r="U2" s="9">
         <v>-65.339265999999995</v>
       </c>
-      <c r="T2" s="10">
+      <c r="V2" s="10">
         <v>6.3950891500000004</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="ALB2"/>
-      <c r="ALC2"/>
       <c r="ALD2"/>
       <c r="ALE2"/>
       <c r="ALF2"/>
@@ -826,8 +846,10 @@
       <c r="AMH2"/>
       <c r="AMI2"/>
       <c r="AMJ2"/>
+      <c r="AMK2"/>
+      <c r="AML2"/>
     </row>
-    <row r="3" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1251</v>
       </c>
@@ -844,56 +866,62 @@
         <v>0.33416994691878599</v>
       </c>
       <c r="F3" s="2">
+        <f t="shared" ref="F3:F47" si="0">B3-D3</f>
+        <v>-0.10484610279681994</v>
+      </c>
+      <c r="G3" s="2">
+        <f t="shared" ref="G3:G47" si="1">C3-E3</f>
+        <v>0.94141462996631398</v>
+      </c>
+      <c r="H3" s="2">
         <v>-1.3260141117014399</v>
       </c>
-      <c r="G3" s="2">
+      <c r="I3" s="2">
         <v>0.80487726190194298</v>
       </c>
-      <c r="H3" s="2">
+      <c r="J3" s="2">
         <v>-4.5434782608695699</v>
       </c>
-      <c r="I3" s="2">
+      <c r="K3" s="2">
         <v>12.438563327032099</v>
       </c>
-      <c r="J3" s="2">
+      <c r="L3" s="2">
         <v>-0.84925741573508895</v>
       </c>
-      <c r="K3" s="2">
+      <c r="M3" s="2">
         <v>3.3688261204329901</v>
       </c>
-      <c r="L3" s="5">
+      <c r="N3" s="5">
         <v>-7.5071547596284498</v>
       </c>
-      <c r="M3" s="1"/>
-      <c r="N3">
+      <c r="O3" s="1"/>
+      <c r="P3">
         <v>14.809717089999999</v>
       </c>
-      <c r="O3">
+      <c r="Q3">
         <v>-27.583543110000001</v>
       </c>
-      <c r="P3" s="9">
+      <c r="R3" s="9">
         <v>28.457619699999999</v>
       </c>
-      <c r="Q3" s="9">
+      <c r="S3" s="9">
         <v>26.5186359</v>
       </c>
-      <c r="R3" s="9">
+      <c r="T3" s="9">
         <v>-76.384567000000004</v>
       </c>
-      <c r="S3" s="9">
+      <c r="U3" s="9">
         <v>-151.88901999999999</v>
       </c>
-      <c r="T3" s="10">
+      <c r="V3" s="10">
         <v>17.331996700000001</v>
       </c>
-      <c r="U3" s="2" t="s">
+      <c r="W3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="2" t="s">
+      <c r="X3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="ALB3"/>
-      <c r="ALC3"/>
       <c r="ALD3"/>
       <c r="ALE3"/>
       <c r="ALF3"/>
@@ -927,8 +955,10 @@
       <c r="AMH3"/>
       <c r="AMI3"/>
       <c r="AMJ3"/>
+      <c r="AMK3"/>
+      <c r="AML3"/>
     </row>
-    <row r="4" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3170</v>
       </c>
@@ -945,56 +975,62 @@
         <v>0.60645754863328705</v>
       </c>
       <c r="F4" s="2">
+        <f t="shared" si="0"/>
+        <v>-4.8074577230470039E-2</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" si="1"/>
+        <v>0.496034831682723</v>
+      </c>
+      <c r="H4" s="2">
         <v>-1.09855425391777</v>
       </c>
-      <c r="G4" s="2">
+      <c r="I4" s="2">
         <v>0.85447496447464899</v>
       </c>
-      <c r="H4" s="2">
+      <c r="J4" s="2">
         <v>-4.5434782608695699</v>
       </c>
-      <c r="I4" s="2">
+      <c r="K4" s="2">
         <v>12.438563327032099</v>
       </c>
-      <c r="J4" s="2">
+      <c r="L4" s="2">
         <v>-1.4278234379200101</v>
       </c>
-      <c r="K4" s="2">
+      <c r="M4" s="2">
         <v>5.9975282647079604</v>
       </c>
-      <c r="L4" s="5">
+      <c r="N4" s="5">
         <v>-14.7036848654447</v>
       </c>
-      <c r="M4" s="1"/>
-      <c r="N4">
+      <c r="O4" s="1"/>
+      <c r="P4">
         <v>7.2056715640000002</v>
       </c>
-      <c r="O4">
+      <c r="Q4">
         <v>7.9489186719999996</v>
       </c>
-      <c r="P4" s="9">
+      <c r="R4" s="9">
         <v>45.655256100000003</v>
       </c>
-      <c r="Q4" s="9">
+      <c r="S4" s="9">
         <v>27.659606799999999</v>
       </c>
-      <c r="R4" s="9">
+      <c r="T4" s="9">
         <v>-84.256866000000002</v>
       </c>
-      <c r="S4" s="9">
+      <c r="U4" s="9">
         <v>11.3170397</v>
       </c>
-      <c r="T4" s="10">
+      <c r="V4" s="10">
         <v>7.12791145</v>
       </c>
-      <c r="U4" s="2" t="s">
+      <c r="W4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V4" s="2" t="s">
+      <c r="X4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="ALB4"/>
-      <c r="ALC4"/>
       <c r="ALD4"/>
       <c r="ALE4"/>
       <c r="ALF4"/>
@@ -1028,8 +1064,10 @@
       <c r="AMH4"/>
       <c r="AMI4"/>
       <c r="AMJ4"/>
+      <c r="AMK4"/>
+      <c r="AML4"/>
     </row>
-    <row r="5" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>3175</v>
       </c>
@@ -1046,56 +1084,62 @@
         <v>-1.4684608153584999</v>
       </c>
       <c r="F5" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.20880836962920321</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0569821686681689</v>
+      </c>
+      <c r="H5" s="2">
         <v>0.175790573915801</v>
       </c>
-      <c r="G5" s="2">
+      <c r="I5" s="2">
         <v>-0.93996973102441606</v>
       </c>
-      <c r="H5" s="2">
+      <c r="J5" s="2">
         <v>-4.5434782608695699</v>
       </c>
-      <c r="I5" s="2">
+      <c r="K5" s="2">
         <v>12.438563327032099</v>
       </c>
-      <c r="J5" s="2">
+      <c r="L5" s="2">
         <v>-1.4278234379200101</v>
       </c>
-      <c r="K5" s="2">
+      <c r="M5" s="2">
         <v>5.9975282647079604</v>
       </c>
-      <c r="L5" s="5">
+      <c r="N5" s="5">
         <v>-14.7036848654447</v>
       </c>
-      <c r="M5" s="1"/>
-      <c r="N5">
+      <c r="O5" s="1"/>
+      <c r="P5">
         <v>82.179938070000006</v>
       </c>
-      <c r="O5">
+      <c r="Q5">
         <v>-52.420184069999998</v>
       </c>
-      <c r="P5" s="9">
+      <c r="R5" s="9">
         <v>7.30699247</v>
       </c>
-      <c r="Q5" s="9">
+      <c r="S5" s="9">
         <v>144.81516099999999</v>
       </c>
-      <c r="R5" s="9">
+      <c r="T5" s="9">
         <v>-128.07988</v>
       </c>
-      <c r="S5" s="9">
+      <c r="U5" s="9">
         <v>-358.61630000000002</v>
       </c>
-      <c r="T5" s="10">
+      <c r="V5" s="10">
         <v>8.4916185100000003</v>
       </c>
-      <c r="U5" s="2" t="s">
+      <c r="W5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V5" s="2" t="s">
+      <c r="X5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="ALB5"/>
-      <c r="ALC5"/>
       <c r="ALD5"/>
       <c r="ALE5"/>
       <c r="ALF5"/>
@@ -1129,8 +1173,10 @@
       <c r="AMH5"/>
       <c r="AMI5"/>
       <c r="AMJ5"/>
+      <c r="AMK5"/>
+      <c r="AML5"/>
     </row>
-    <row r="6" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>1015</v>
       </c>
@@ -1147,56 +1193,62 @@
         <v>1.3497740606411199</v>
       </c>
       <c r="F6" s="2">
+        <f t="shared" si="0"/>
+        <v>-5.0197267071721008E-2</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.47129038980028293</v>
+      </c>
+      <c r="H6" s="2">
         <v>-0.29255640792610699</v>
       </c>
-      <c r="G6" s="2">
+      <c r="I6" s="2">
         <v>1.11412886574098</v>
       </c>
-      <c r="H6" s="2">
+      <c r="J6" s="2">
         <v>-3.5434782608695699</v>
       </c>
-      <c r="I6" s="2">
+      <c r="K6" s="2">
         <v>4.3516068052930104</v>
       </c>
-      <c r="J6" s="2">
+      <c r="L6" s="2">
         <v>2.3328557062819901</v>
       </c>
-      <c r="K6" s="2">
+      <c r="M6" s="2">
         <v>-8.7561799667974007</v>
       </c>
-      <c r="L6" s="5">
+      <c r="N6" s="5">
         <v>13.2080581541674</v>
       </c>
-      <c r="M6" s="1"/>
-      <c r="N6">
+      <c r="O6" s="1"/>
+      <c r="P6">
         <v>137.5536429</v>
       </c>
-      <c r="O6">
+      <c r="Q6">
         <v>-37.040660770000002</v>
       </c>
-      <c r="P6" s="9">
+      <c r="R6" s="9">
         <v>9.8110612899999996</v>
       </c>
-      <c r="Q6" s="9">
+      <c r="S6" s="9">
         <v>8.7763971200000004</v>
       </c>
-      <c r="R6" s="9">
+      <c r="T6" s="9">
         <v>-3.2836219999999998</v>
       </c>
-      <c r="S6" s="9">
+      <c r="U6" s="9">
         <v>-78.666763000000003</v>
       </c>
-      <c r="T6" s="10">
+      <c r="V6" s="10">
         <v>6.2024719700000004</v>
       </c>
-      <c r="U6" s="2" t="s">
+      <c r="W6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V6" s="2" t="s">
+      <c r="X6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="ALB6"/>
-      <c r="ALC6"/>
       <c r="ALD6"/>
       <c r="ALE6"/>
       <c r="ALF6"/>
@@ -1230,8 +1282,10 @@
       <c r="AMH6"/>
       <c r="AMI6"/>
       <c r="AMJ6"/>
+      <c r="AMK6"/>
+      <c r="AML6"/>
     </row>
-    <row r="7" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>3166</v>
       </c>
@@ -1248,56 +1302,62 @@
         <v>1.04787921122765</v>
       </c>
       <c r="F7" s="2">
+        <f t="shared" si="0"/>
+        <v>3.7091968286149801E-3</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.72777832650762497</v>
+      </c>
+      <c r="H7" s="2">
         <v>-0.35407376752598402</v>
       </c>
-      <c r="G7" s="2">
+      <c r="I7" s="2">
         <v>0.683990047973838</v>
       </c>
-      <c r="H7" s="2">
+      <c r="J7" s="2">
         <v>-3.5434782608695699</v>
       </c>
-      <c r="I7" s="2">
+      <c r="K7" s="2">
         <v>4.3516068052930104</v>
       </c>
-      <c r="J7" s="2">
+      <c r="L7" s="2">
         <v>-0.41823128913277902</v>
       </c>
-      <c r="K7" s="2">
+      <c r="M7" s="2">
         <v>0.992236995215804</v>
       </c>
-      <c r="L7" s="5">
+      <c r="N7" s="5">
         <v>1.2364092629674399</v>
       </c>
-      <c r="M7" s="1"/>
-      <c r="N7">
+      <c r="O7" s="1"/>
+      <c r="P7">
         <v>-10.141561340000001</v>
       </c>
-      <c r="O7">
+      <c r="Q7">
         <v>-6.0681958199999997</v>
       </c>
-      <c r="P7" s="9">
+      <c r="R7" s="9">
         <v>69.3166899</v>
       </c>
-      <c r="Q7" s="9">
+      <c r="S7" s="9">
         <v>1.1984495100000001</v>
       </c>
-      <c r="R7" s="9">
+      <c r="T7" s="9">
         <v>-44.105659000000003</v>
       </c>
-      <c r="S7" s="9">
+      <c r="U7" s="9">
         <v>-82.397115999999997</v>
       </c>
-      <c r="T7" s="10">
+      <c r="V7" s="10">
         <v>-20.147648799999999</v>
       </c>
-      <c r="U7" s="2" t="s">
+      <c r="W7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V7" s="2" t="s">
+      <c r="X7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="ALB7"/>
-      <c r="ALC7"/>
       <c r="ALD7"/>
       <c r="ALE7"/>
       <c r="ALF7"/>
@@ -1331,8 +1391,10 @@
       <c r="AMH7"/>
       <c r="AMI7"/>
       <c r="AMJ7"/>
+      <c r="AMK7"/>
+      <c r="AML7"/>
     </row>
-    <row r="8" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>3176</v>
       </c>
@@ -1349,56 +1411,62 @@
         <v>-1.6552463304318099</v>
       </c>
       <c r="F8" s="2">
+        <f t="shared" si="0"/>
+        <v>-1.4699889704978868</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="1"/>
+        <v>1.938758705089731</v>
+      </c>
+      <c r="H8" s="2">
         <v>1.0319507540364801</v>
       </c>
-      <c r="G8" s="2">
+      <c r="I8" s="2">
         <v>-0.68586697788694395</v>
       </c>
-      <c r="H8" s="2">
+      <c r="J8" s="2">
         <v>-3.5434782608695699</v>
       </c>
-      <c r="I8" s="2">
+      <c r="K8" s="2">
         <v>4.3516068052930104</v>
       </c>
-      <c r="J8" s="2">
+      <c r="L8" s="2">
         <v>0.66513080744576103</v>
       </c>
-      <c r="K8" s="2">
+      <c r="M8" s="2">
         <v>-2.8466330426603301</v>
       </c>
-      <c r="L8" s="5">
+      <c r="N8" s="5">
         <v>5.9507751350351201</v>
       </c>
-      <c r="M8" s="1"/>
-      <c r="N8">
+      <c r="O8" s="1"/>
+      <c r="P8">
         <v>47.39930528</v>
       </c>
-      <c r="O8">
+      <c r="Q8">
         <v>-7.1413466720000001</v>
       </c>
-      <c r="P8" s="9">
+      <c r="R8" s="9">
         <v>6.3353449199999998</v>
       </c>
-      <c r="Q8" s="9">
+      <c r="S8" s="9">
         <v>97.178318599999997</v>
       </c>
-      <c r="R8" s="9">
+      <c r="T8" s="9">
         <v>44.9247704</v>
       </c>
-      <c r="S8" s="9">
+      <c r="U8" s="9">
         <v>-6.6006711999999998</v>
       </c>
-      <c r="T8" s="10">
+      <c r="V8" s="10">
         <v>1.61933613</v>
       </c>
-      <c r="U8" s="2" t="s">
+      <c r="W8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V8" s="2" t="s">
+      <c r="X8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="ALB8"/>
-      <c r="ALC8"/>
       <c r="ALD8"/>
       <c r="ALE8"/>
       <c r="ALF8"/>
@@ -1432,8 +1500,10 @@
       <c r="AMH8"/>
       <c r="AMI8"/>
       <c r="AMJ8"/>
+      <c r="AMK8"/>
+      <c r="AML8"/>
     </row>
-    <row r="9" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>3200</v>
       </c>
@@ -1450,56 +1520,62 @@
         <v>0.130621233287534</v>
       </c>
       <c r="F9" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.14276554080047602</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="1"/>
+        <v>0.40501128325352104</v>
+      </c>
+      <c r="H9" s="2">
         <v>-0.24378501152425999</v>
       </c>
-      <c r="G9" s="2">
+      <c r="I9" s="2">
         <v>0.33312687491429399</v>
       </c>
-      <c r="H9" s="2">
+      <c r="J9" s="2">
         <v>-3.5434782608695699</v>
       </c>
-      <c r="I9" s="2">
+      <c r="K9" s="2">
         <v>4.3516068052930104</v>
       </c>
-      <c r="J9" s="2">
+      <c r="L9" s="2">
         <v>-1.4278234379200101</v>
       </c>
-      <c r="K9" s="2">
+      <c r="M9" s="2">
         <v>4.5697048267879499</v>
       </c>
-      <c r="L9" s="5">
+      <c r="N9" s="5">
         <v>-3.1569388022654601</v>
       </c>
-      <c r="M9" s="1"/>
-      <c r="N9">
+      <c r="O9" s="1"/>
+      <c r="P9">
         <v>-39.167937070000001</v>
       </c>
-      <c r="O9">
+      <c r="Q9">
         <v>-10.59996668</v>
       </c>
-      <c r="P9" s="9">
+      <c r="R9" s="9">
         <v>-10.433695999999999</v>
       </c>
-      <c r="Q9" s="9">
+      <c r="S9" s="9">
         <v>134.91744399999999</v>
       </c>
-      <c r="R9" s="9">
+      <c r="T9" s="9">
         <v>28.379520400000001</v>
       </c>
-      <c r="S9" s="9">
+      <c r="U9" s="9">
         <v>25.4298669</v>
       </c>
-      <c r="T9" s="10">
+      <c r="V9" s="10">
         <v>4.15968275</v>
       </c>
-      <c r="U9" s="2" t="s">
+      <c r="W9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V9" s="2" t="s">
+      <c r="X9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="ALB9"/>
-      <c r="ALC9"/>
       <c r="ALD9"/>
       <c r="ALE9"/>
       <c r="ALF9"/>
@@ -1533,8 +1609,10 @@
       <c r="AMH9"/>
       <c r="AMI9"/>
       <c r="AMJ9"/>
+      <c r="AMK9"/>
+      <c r="AML9"/>
     </row>
-    <row r="10" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>3212</v>
       </c>
@@ -1551,56 +1629,62 @@
         <v>0.68661641149998998</v>
       </c>
       <c r="F10" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.21391574560518012</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="1"/>
+        <v>0.46131001309899</v>
+      </c>
+      <c r="H10" s="2">
         <v>-1.4981282435650101</v>
       </c>
-      <c r="G10" s="2">
+      <c r="I10" s="2">
         <v>0.91727141804948498</v>
       </c>
-      <c r="H10" s="2">
+      <c r="J10" s="2">
         <v>-3.5434782608695699</v>
       </c>
-      <c r="I10" s="2">
+      <c r="K10" s="2">
         <v>4.3516068052930104</v>
       </c>
-      <c r="J10" s="2">
+      <c r="L10" s="2">
         <v>-1.4278234379200101</v>
       </c>
-      <c r="K10" s="2">
+      <c r="M10" s="2">
         <v>4.5697048267879499</v>
       </c>
-      <c r="L10" s="5">
+      <c r="N10" s="5">
         <v>-3.1569388022654601</v>
       </c>
-      <c r="M10" s="1"/>
-      <c r="N10">
+      <c r="O10" s="1"/>
+      <c r="P10">
         <v>-42.168360450000002</v>
       </c>
-      <c r="O10">
+      <c r="Q10">
         <v>-42.49175529</v>
       </c>
-      <c r="P10" s="9">
+      <c r="R10" s="9">
         <v>13.6012694</v>
       </c>
-      <c r="Q10" s="9">
+      <c r="S10" s="9">
         <v>70.448237700000007</v>
       </c>
-      <c r="R10" s="9">
+      <c r="T10" s="9">
         <v>-60.202933999999999</v>
       </c>
-      <c r="S10" s="9">
+      <c r="U10" s="9">
         <v>2.5042821599999998</v>
       </c>
-      <c r="T10" s="10">
+      <c r="V10" s="10">
         <v>5.350276</v>
       </c>
-      <c r="U10" s="2" t="s">
+      <c r="W10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V10" s="2" t="s">
+      <c r="X10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="ALB10"/>
-      <c r="ALC10"/>
       <c r="ALD10"/>
       <c r="ALE10"/>
       <c r="ALF10"/>
@@ -1634,8 +1718,10 @@
       <c r="AMH10"/>
       <c r="AMI10"/>
       <c r="AMJ10"/>
+      <c r="AMK10"/>
+      <c r="AML10"/>
     </row>
-    <row r="11" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>1245</v>
       </c>
@@ -1652,56 +1738,62 @@
         <v>0.220742567604582</v>
       </c>
       <c r="F11" s="2">
+        <f t="shared" si="0"/>
+        <v>7.2344512487430013E-2</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="1"/>
+        <v>0.114896971798153</v>
+      </c>
+      <c r="H11" s="2">
         <v>-1.0641983451844601</v>
       </c>
-      <c r="G11" s="2">
+      <c r="I11" s="2">
         <v>0.27819105350365902</v>
       </c>
-      <c r="H11" s="2">
+      <c r="J11" s="2">
         <v>-2.5434782608695699</v>
       </c>
-      <c r="I11" s="2">
+      <c r="K11" s="2">
         <v>-1.73534971644612</v>
       </c>
-      <c r="J11" s="2">
+      <c r="L11" s="2">
         <v>0.16033473305214499</v>
       </c>
-      <c r="K11" s="2">
+      <c r="M11" s="2">
         <v>-0.89756439382210795</v>
       </c>
-      <c r="L11" s="5">
+      <c r="N11" s="5">
         <v>2.7781505534056099</v>
       </c>
-      <c r="M11" s="1"/>
-      <c r="N11">
+      <c r="O11" s="1"/>
+      <c r="P11">
         <v>15.33062898</v>
       </c>
-      <c r="O11">
+      <c r="Q11">
         <v>-34.288015459999997</v>
       </c>
-      <c r="P11" s="9">
+      <c r="R11" s="9">
         <v>30.846215300000001</v>
       </c>
-      <c r="Q11" s="9">
+      <c r="S11" s="9">
         <v>19.662128599999999</v>
       </c>
-      <c r="R11" s="9">
+      <c r="T11" s="9">
         <v>-37.565967999999998</v>
       </c>
-      <c r="S11" s="9">
+      <c r="U11" s="9">
         <v>-13.801031</v>
       </c>
-      <c r="T11" s="10">
+      <c r="V11" s="10">
         <v>-0.52523613000000002</v>
       </c>
-      <c r="U11" s="2" t="s">
+      <c r="W11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V11" s="2" t="s">
+      <c r="X11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="ALB11"/>
-      <c r="ALC11"/>
       <c r="ALD11"/>
       <c r="ALE11"/>
       <c r="ALF11"/>
@@ -1735,8 +1827,10 @@
       <c r="AMH11"/>
       <c r="AMI11"/>
       <c r="AMJ11"/>
+      <c r="AMK11"/>
+      <c r="AML11"/>
     </row>
-    <row r="12" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>1276</v>
       </c>
@@ -1753,56 +1847,62 @@
         <v>0.351136584670664</v>
       </c>
       <c r="F12" s="2">
+        <f t="shared" si="0"/>
+        <v>9.6222679860088034E-2</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.65388498682861207</v>
+      </c>
+      <c r="H12" s="2">
         <v>-0.41289670606027401</v>
       </c>
-      <c r="G12" s="2">
+      <c r="I12" s="2">
         <v>2.4194091256358002E-2</v>
       </c>
-      <c r="H12" s="2">
+      <c r="J12" s="2">
         <v>-2.5434782608695699</v>
       </c>
-      <c r="I12" s="2">
+      <c r="K12" s="2">
         <v>-1.73534971644612</v>
       </c>
-      <c r="J12" s="2">
+      <c r="L12" s="2">
         <v>-1.4278234379200101</v>
       </c>
-      <c r="K12" s="2">
+      <c r="M12" s="2">
         <v>3.1418813888679402</v>
       </c>
-      <c r="L12" s="5">
+      <c r="N12" s="5">
         <v>5.5341603850737302</v>
       </c>
-      <c r="M12" s="1"/>
-      <c r="N12">
+      <c r="O12" s="1"/>
+      <c r="P12">
         <v>-18.511118809999999</v>
       </c>
-      <c r="O12">
+      <c r="Q12">
         <v>-58.791950059999998</v>
       </c>
-      <c r="P12" s="9">
+      <c r="R12" s="9">
         <v>-94.775426999999993</v>
       </c>
-      <c r="Q12" s="9">
+      <c r="S12" s="9">
         <v>22.9194055</v>
       </c>
-      <c r="R12" s="9">
+      <c r="T12" s="9">
         <v>-4.0706252999999997</v>
       </c>
-      <c r="S12" s="9">
+      <c r="U12" s="9">
         <v>9.0527590500000006</v>
       </c>
-      <c r="T12" s="10">
+      <c r="V12" s="10">
         <v>3.8040723399999998</v>
       </c>
-      <c r="U12" s="2" t="s">
+      <c r="W12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V12" s="2" t="s">
+      <c r="X12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="ALB12"/>
-      <c r="ALC12"/>
       <c r="ALD12"/>
       <c r="ALE12"/>
       <c r="ALF12"/>
@@ -1836,8 +1936,10 @@
       <c r="AMH12"/>
       <c r="AMI12"/>
       <c r="AMJ12"/>
+      <c r="AMK12"/>
+      <c r="AML12"/>
     </row>
-    <row r="13" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>1294</v>
       </c>
@@ -1854,56 +1956,62 @@
         <v>0.461805595946847</v>
       </c>
       <c r="F13" s="2">
+        <f t="shared" si="0"/>
+        <v>0.14987478882537497</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.68363835943151496</v>
+      </c>
+      <c r="H13" s="2">
         <v>-0.72467976382863297</v>
       </c>
-      <c r="G13" s="2">
+      <c r="I13" s="2">
         <v>0.11998641623109001</v>
       </c>
-      <c r="H13" s="2">
+      <c r="J13" s="2">
         <v>-2.5434782608695699</v>
       </c>
-      <c r="I13" s="2">
+      <c r="K13" s="2">
         <v>-1.73534971644612</v>
       </c>
-      <c r="J13" s="2">
+      <c r="L13" s="2">
         <v>-1.1385404268275501</v>
       </c>
-      <c r="K13" s="2">
+      <c r="M13" s="2">
         <v>2.40609633891538</v>
       </c>
-      <c r="L13" s="5">
+      <c r="N13" s="5">
         <v>5.0321531938017499</v>
       </c>
-      <c r="M13" s="1"/>
-      <c r="N13">
+      <c r="O13" s="1"/>
+      <c r="P13">
         <v>41.22765502</v>
       </c>
-      <c r="O13">
+      <c r="Q13">
         <v>-43.504668459999998</v>
       </c>
-      <c r="P13" s="9">
+      <c r="R13" s="9">
         <v>-6.5267790000000003</v>
       </c>
-      <c r="Q13" s="9">
+      <c r="S13" s="9">
         <v>60.975080200000001</v>
       </c>
-      <c r="R13" s="9">
+      <c r="T13" s="9">
         <v>-31.702311000000002</v>
       </c>
-      <c r="S13" s="9">
+      <c r="U13" s="9">
         <v>-14.529658</v>
       </c>
-      <c r="T13" s="10">
+      <c r="V13" s="10">
         <v>6.85294282</v>
       </c>
-      <c r="U13" s="2" t="s">
+      <c r="W13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V13" s="2" t="s">
+      <c r="X13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="ALB13"/>
-      <c r="ALC13"/>
       <c r="ALD13"/>
       <c r="ALE13"/>
       <c r="ALF13"/>
@@ -1937,8 +2045,10 @@
       <c r="AMH13"/>
       <c r="AMI13"/>
       <c r="AMJ13"/>
+      <c r="AMK13"/>
+      <c r="AML13"/>
     </row>
-    <row r="14" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>1301</v>
       </c>
@@ -1955,56 +2065,62 @@
         <v>0.32900851309694701</v>
       </c>
       <c r="F14" s="2">
+        <f t="shared" si="0"/>
+        <v>0.30172533487513997</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="1"/>
+        <v>-1.016612375823845</v>
+      </c>
+      <c r="H14" s="2">
         <v>0.87214832999455005</v>
       </c>
-      <c r="G14" s="2">
+      <c r="I14" s="2">
         <v>-0.17929767481497599</v>
       </c>
-      <c r="H14" s="2">
+      <c r="J14" s="2">
         <v>-2.5434782608695699</v>
       </c>
-      <c r="I14" s="2">
+      <c r="K14" s="2">
         <v>-1.73534971644612</v>
       </c>
-      <c r="J14" s="2">
+      <c r="L14" s="2">
         <v>1.85916175422969E-2</v>
       </c>
-      <c r="K14" s="2">
+      <c r="M14" s="2">
         <v>-0.53704386089488598</v>
       </c>
-      <c r="L14" s="5">
+      <c r="N14" s="5">
         <v>3.0241244287138098</v>
       </c>
-      <c r="M14" s="1"/>
-      <c r="N14">
+      <c r="O14" s="1"/>
+      <c r="P14">
         <v>20.289118040000002</v>
       </c>
-      <c r="O14">
+      <c r="Q14">
         <v>-52.688322890000002</v>
       </c>
-      <c r="P14" s="9">
+      <c r="R14" s="9">
         <v>-39.719687999999998</v>
       </c>
-      <c r="Q14" s="9">
+      <c r="S14" s="9">
         <v>85.316176999999996</v>
       </c>
-      <c r="R14" s="9">
+      <c r="T14" s="9">
         <v>44.038662000000002</v>
       </c>
-      <c r="S14" s="9">
+      <c r="U14" s="9">
         <v>131.42799500000001</v>
       </c>
-      <c r="T14" s="10">
+      <c r="V14" s="10">
         <v>14.641844300000001</v>
       </c>
-      <c r="U14" s="2" t="s">
+      <c r="W14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V14" s="2" t="s">
+      <c r="X14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="ALB14"/>
-      <c r="ALC14"/>
       <c r="ALD14"/>
       <c r="ALE14"/>
       <c r="ALF14"/>
@@ -2038,8 +2154,10 @@
       <c r="AMH14"/>
       <c r="AMI14"/>
       <c r="AMJ14"/>
+      <c r="AMK14"/>
+      <c r="AML14"/>
     </row>
-    <row r="15" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>3167</v>
       </c>
@@ -2056,56 +2174,62 @@
         <v>0.3085684456019</v>
       </c>
       <c r="F15" s="2">
+        <f t="shared" si="0"/>
+        <v>0.3621651563609723</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="1"/>
+        <v>0.27603014502404299</v>
+      </c>
+      <c r="H15" s="2">
         <v>0.23185696761928301</v>
       </c>
-      <c r="G15" s="2">
+      <c r="I15" s="2">
         <v>0.446583518113922</v>
       </c>
-      <c r="H15" s="2">
+      <c r="J15" s="2">
         <v>-2.5434782608695699</v>
       </c>
-      <c r="I15" s="2">
+      <c r="K15" s="2">
         <v>-1.73534971644612</v>
       </c>
-      <c r="J15" s="2">
+      <c r="L15" s="2">
         <v>-1.1385404268275501</v>
       </c>
-      <c r="K15" s="2">
+      <c r="M15" s="2">
         <v>2.40609633891538</v>
       </c>
-      <c r="L15" s="5">
+      <c r="N15" s="5">
         <v>5.0321531938017499</v>
       </c>
-      <c r="M15" s="1"/>
-      <c r="N15">
+      <c r="O15" s="1"/>
+      <c r="P15">
         <v>1.587598729</v>
       </c>
-      <c r="O15">
+      <c r="Q15">
         <v>-2.7098392869999999</v>
       </c>
-      <c r="P15" s="9">
+      <c r="R15" s="9">
         <v>48.249327299999997</v>
       </c>
-      <c r="Q15" s="9">
+      <c r="S15" s="9">
         <v>50.172426799999997</v>
       </c>
-      <c r="R15" s="9">
+      <c r="T15" s="9">
         <v>12.237022400000001</v>
       </c>
-      <c r="S15" s="9">
+      <c r="U15" s="9">
         <v>-58.242565999999997</v>
       </c>
-      <c r="T15" s="10">
+      <c r="V15" s="10">
         <v>6.7484929600000001</v>
       </c>
-      <c r="U15" s="2" t="s">
+      <c r="W15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V15" s="2" t="s">
+      <c r="X15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="ALB15"/>
-      <c r="ALC15"/>
       <c r="ALD15"/>
       <c r="ALE15"/>
       <c r="ALF15"/>
@@ -2139,8 +2263,10 @@
       <c r="AMH15"/>
       <c r="AMI15"/>
       <c r="AMJ15"/>
+      <c r="AMK15"/>
+      <c r="AML15"/>
     </row>
-    <row r="16" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>1010</v>
       </c>
@@ -2157,56 +2283,62 @@
         <v>-2.1221013943518199</v>
       </c>
       <c r="F16" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.24392858358691982</v>
+      </c>
+      <c r="G16" s="2">
+        <f t="shared" si="1"/>
+        <v>0.17971044844360984</v>
+      </c>
+      <c r="H16" s="2">
         <v>1.99055132549833</v>
       </c>
-      <c r="G16" s="2">
+      <c r="I16" s="2">
         <v>-2.0322461701300099</v>
       </c>
-      <c r="H16" s="2">
+      <c r="J16" s="2">
         <v>-1.5434782608695701</v>
       </c>
-      <c r="I16" s="2">
+      <c r="K16" s="2">
         <v>-5.8223062381852504</v>
       </c>
-      <c r="J16" s="2">
+      <c r="L16" s="2">
         <v>3.4841909705790699</v>
       </c>
-      <c r="K16" s="2">
+      <c r="M16" s="2">
         <v>-5.8675295056484797</v>
       </c>
-      <c r="L16" s="5">
+      <c r="N16" s="5">
         <v>-17.229639436087101</v>
       </c>
-      <c r="M16" s="1"/>
-      <c r="N16">
+      <c r="O16" s="1"/>
+      <c r="P16">
         <v>136.85611660000001</v>
       </c>
-      <c r="O16">
+      <c r="Q16">
         <v>1.2653025339999999</v>
       </c>
-      <c r="P16" s="9">
+      <c r="R16" s="9">
         <v>73.222070900000006</v>
       </c>
-      <c r="Q16" s="9">
+      <c r="S16" s="9">
         <v>61.411937299999998</v>
       </c>
-      <c r="R16" s="9">
+      <c r="T16" s="9">
         <v>1.0866508500000001</v>
       </c>
-      <c r="S16" s="9">
+      <c r="U16" s="9">
         <v>60.556766600000003</v>
       </c>
-      <c r="T16" s="10">
+      <c r="V16" s="10">
         <v>-8.2675678099999992</v>
       </c>
-      <c r="U16" s="2" t="s">
+      <c r="W16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V16" s="2" t="s">
+      <c r="X16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="ALB16"/>
-      <c r="ALC16"/>
       <c r="ALD16"/>
       <c r="ALE16"/>
       <c r="ALF16"/>
@@ -2240,8 +2372,10 @@
       <c r="AMH16"/>
       <c r="AMI16"/>
       <c r="AMJ16"/>
+      <c r="AMK16"/>
+      <c r="AML16"/>
     </row>
-    <row r="17" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>1021</v>
       </c>
@@ -2258,56 +2392,62 @@
         <v>-0.79263613146103995</v>
       </c>
       <c r="F17" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.52633852382324198</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" si="1"/>
+        <v>1.570859420889462</v>
+      </c>
+      <c r="H17" s="2">
         <v>0.160388132576642</v>
       </c>
-      <c r="G17" s="2">
+      <c r="I17" s="2">
         <v>-7.2064210163089197E-3</v>
       </c>
-      <c r="H17" s="2">
+      <c r="J17" s="2">
         <v>-1.5434782608695701</v>
       </c>
-      <c r="I17" s="2">
+      <c r="K17" s="2">
         <v>-5.8223062381852504</v>
       </c>
-      <c r="J17" s="2">
+      <c r="L17" s="2">
         <v>-0.55997440464262704</v>
       </c>
-      <c r="K17" s="2">
+      <c r="M17" s="2">
         <v>0.37455183436762002</v>
       </c>
-      <c r="L17" s="5">
+      <c r="N17" s="5">
         <v>6.3167298563189496</v>
       </c>
-      <c r="M17" s="1"/>
-      <c r="N17">
+      <c r="O17" s="1"/>
+      <c r="P17">
         <v>24.766350419999998</v>
       </c>
-      <c r="O17">
+      <c r="Q17">
         <v>-20.46612571</v>
       </c>
-      <c r="P17" s="9">
+      <c r="R17" s="9">
         <v>-51.911189</v>
       </c>
-      <c r="Q17" s="9">
+      <c r="S17" s="9">
         <v>68.3805835</v>
       </c>
-      <c r="R17" s="9">
+      <c r="T17" s="9">
         <v>-15.590310000000001</v>
       </c>
-      <c r="S17" s="9">
+      <c r="U17" s="9">
         <v>-44.462949999999999</v>
       </c>
-      <c r="T17" s="10">
+      <c r="V17" s="10">
         <v>5.7089557700000002</v>
       </c>
-      <c r="U17" s="2" t="s">
+      <c r="W17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V17" s="2" t="s">
+      <c r="X17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="ALB17"/>
-      <c r="ALC17"/>
       <c r="ALD17"/>
       <c r="ALE17"/>
       <c r="ALF17"/>
@@ -2341,8 +2481,10 @@
       <c r="AMH17"/>
       <c r="AMI17"/>
       <c r="AMJ17"/>
+      <c r="AMK17"/>
+      <c r="AML17"/>
     </row>
-    <row r="18" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>1243</v>
       </c>
@@ -2359,56 +2501,62 @@
         <v>0.158890685222914</v>
       </c>
       <c r="F18" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.17662958418405994</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="shared" si="1"/>
+        <v>0.13457001673671998</v>
+      </c>
+      <c r="H18" s="2">
         <v>2.4116615790065299</v>
       </c>
-      <c r="G18" s="2">
+      <c r="I18" s="2">
         <v>0.22617569359127401</v>
       </c>
-      <c r="H18" s="2">
+      <c r="J18" s="2">
         <v>-1.5434782608695701</v>
       </c>
-      <c r="I18" s="2">
+      <c r="K18" s="2">
         <v>-5.8223062381852504</v>
       </c>
-      <c r="J18" s="2">
+      <c r="L18" s="2">
         <v>-0.55997440464262704</v>
       </c>
-      <c r="K18" s="2">
+      <c r="M18" s="2">
         <v>0.37455183436762002</v>
       </c>
-      <c r="L18" s="5">
+      <c r="N18" s="5">
         <v>6.3167298563189496</v>
       </c>
-      <c r="M18" s="1"/>
-      <c r="N18">
+      <c r="O18" s="1"/>
+      <c r="P18">
         <v>-19.063366630000001</v>
       </c>
-      <c r="O18">
+      <c r="Q18">
         <v>-11.88032216</v>
       </c>
-      <c r="P18" s="9">
+      <c r="R18" s="9">
         <v>-11.570719</v>
       </c>
-      <c r="Q18" s="9">
+      <c r="S18" s="9">
         <v>28.1792041</v>
       </c>
-      <c r="R18" s="9">
+      <c r="T18" s="9">
         <v>68.790626500000002</v>
       </c>
-      <c r="S18" s="9">
+      <c r="U18" s="9">
         <v>55.120243299999998</v>
       </c>
-      <c r="T18" s="10">
+      <c r="V18" s="10">
         <v>5.8634147700000003</v>
       </c>
-      <c r="U18" s="2" t="s">
+      <c r="W18" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V18" s="2" t="s">
+      <c r="X18" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="ALB18"/>
-      <c r="ALC18"/>
       <c r="ALD18"/>
       <c r="ALE18"/>
       <c r="ALF18"/>
@@ -2442,8 +2590,10 @@
       <c r="AMH18"/>
       <c r="AMI18"/>
       <c r="AMJ18"/>
+      <c r="AMK18"/>
+      <c r="AML18"/>
     </row>
-    <row r="19" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>3140</v>
       </c>
@@ -2460,56 +2610,62 @@
         <v>0.72433002657940004</v>
       </c>
       <c r="F19" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15990369254783818</v>
+      </c>
+      <c r="G19" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.87614934317504201</v>
+      </c>
+      <c r="H19" s="2">
         <v>7.7583161815272902E-2</v>
       </c>
-      <c r="G19" s="2">
+      <c r="I19" s="2">
         <v>0.28625535499187899</v>
       </c>
-      <c r="H19" s="2">
+      <c r="J19" s="2">
         <v>-1.5434782608695701</v>
       </c>
-      <c r="I19" s="2">
+      <c r="K19" s="2">
         <v>-5.8223062381852504</v>
       </c>
-      <c r="J19" s="2">
+      <c r="L19" s="2">
         <v>0.17930440161112399</v>
       </c>
-      <c r="K19" s="2">
+      <c r="M19" s="2">
         <v>-0.76650893180664803</v>
       </c>
-      <c r="L19" s="5">
+      <c r="N19" s="5">
         <v>2.0124222509095899</v>
       </c>
-      <c r="M19" s="1"/>
-      <c r="N19">
+      <c r="O19" s="1"/>
+      <c r="P19">
         <v>41.97258978</v>
       </c>
-      <c r="O19">
+      <c r="Q19">
         <v>-13.56885458</v>
       </c>
-      <c r="P19" s="9">
+      <c r="R19" s="9">
         <v>-41.793593000000001</v>
       </c>
-      <c r="Q19" s="9">
+      <c r="S19" s="9">
         <v>-7.4376822999999996</v>
       </c>
-      <c r="R19" s="9">
+      <c r="T19" s="9">
         <v>44.8323441</v>
       </c>
-      <c r="S19" s="9">
+      <c r="U19" s="9">
         <v>10.9789168</v>
       </c>
-      <c r="T19" s="10">
+      <c r="V19" s="10">
         <v>-9.1280710700000007</v>
       </c>
-      <c r="U19" s="2" t="s">
+      <c r="W19" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V19" s="2" t="s">
+      <c r="X19" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="ALB19"/>
-      <c r="ALC19"/>
       <c r="ALD19"/>
       <c r="ALE19"/>
       <c r="ALF19"/>
@@ -2543,8 +2699,10 @@
       <c r="AMH19"/>
       <c r="AMI19"/>
       <c r="AMJ19"/>
+      <c r="AMK19"/>
+      <c r="AML19"/>
     </row>
-    <row r="20" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>1003</v>
       </c>
@@ -2561,56 +2719,62 @@
         <v>-0.39969206278992198</v>
       </c>
       <c r="F20" s="2">
+        <f t="shared" si="0"/>
+        <v>1.354368093639692</v>
+      </c>
+      <c r="G20" s="2">
+        <f t="shared" si="1"/>
+        <v>-1.046190672054998</v>
+      </c>
+      <c r="H20" s="2">
         <v>1.2150853835381299</v>
       </c>
-      <c r="G20" s="2">
+      <c r="I20" s="2">
         <v>-0.922787398817421</v>
       </c>
-      <c r="H20" s="2">
+      <c r="J20" s="2">
         <v>-0.54347826086956597</v>
       </c>
-      <c r="I20" s="2">
+      <c r="K20" s="2">
         <v>-7.9092627599243901</v>
       </c>
-      <c r="J20" s="2">
+      <c r="L20" s="2">
         <v>1.85916175422969E-2</v>
       </c>
-      <c r="K20" s="2">
+      <c r="M20" s="2">
         <v>-0.499860625810292</v>
       </c>
-      <c r="L20" s="5">
+      <c r="N20" s="5">
         <v>2.9093413986700698</v>
       </c>
-      <c r="M20" s="1"/>
-      <c r="N20">
+      <c r="O20" s="1"/>
+      <c r="P20">
         <v>12.90129531</v>
       </c>
-      <c r="O20">
+      <c r="Q20">
         <v>-15.89482918</v>
       </c>
-      <c r="P20" s="9">
+      <c r="R20" s="9">
         <v>113.864529</v>
       </c>
-      <c r="Q20" s="9">
+      <c r="S20" s="9">
         <v>-12.325996999999999</v>
       </c>
-      <c r="R20" s="9">
+      <c r="T20" s="9">
         <v>24.9903297</v>
       </c>
-      <c r="S20" s="9">
+      <c r="U20" s="9">
         <v>61.768232400000002</v>
       </c>
-      <c r="T20" s="10">
+      <c r="V20" s="10">
         <v>-4.7663415699999998</v>
       </c>
-      <c r="U20" s="2" t="s">
+      <c r="W20" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V20" s="2" t="s">
+      <c r="X20" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="ALB20"/>
-      <c r="ALC20"/>
       <c r="ALD20"/>
       <c r="ALE20"/>
       <c r="ALF20"/>
@@ -2644,8 +2808,10 @@
       <c r="AMH20"/>
       <c r="AMI20"/>
       <c r="AMJ20"/>
+      <c r="AMK20"/>
+      <c r="AML20"/>
     </row>
-    <row r="21" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>1006</v>
       </c>
@@ -2662,56 +2828,62 @@
         <v>-0.72377562558110198</v>
       </c>
       <c r="F21" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.29681935977529605</v>
+      </c>
+      <c r="G21" s="2">
+        <f t="shared" si="1"/>
+        <v>1.8553621609243121</v>
+      </c>
+      <c r="H21" s="2">
         <v>-0.72754522851702197</v>
       </c>
-      <c r="G21" s="2">
+      <c r="I21" s="2">
         <v>0.20390545488105399</v>
       </c>
-      <c r="H21" s="2">
+      <c r="J21" s="2">
         <v>-0.54347826086956597</v>
       </c>
-      <c r="I21" s="2">
+      <c r="K21" s="2">
         <v>-7.9092627599243901</v>
       </c>
-      <c r="J21" s="2">
+      <c r="L21" s="2">
         <v>-1.1385404268275501</v>
       </c>
-      <c r="K21" s="2">
+      <c r="M21" s="2">
         <v>0.12901548526027701</v>
       </c>
-      <c r="L21" s="5">
+      <c r="N21" s="5">
         <v>12.0614027855197</v>
       </c>
-      <c r="M21" s="1"/>
-      <c r="N21">
+      <c r="O21" s="1"/>
+      <c r="P21">
         <v>21.993202879999998</v>
       </c>
-      <c r="O21">
+      <c r="Q21">
         <v>-15.71320637</v>
       </c>
-      <c r="P21" s="9">
+      <c r="R21" s="9">
         <v>46.251495400000003</v>
       </c>
-      <c r="Q21" s="9">
+      <c r="S21" s="9">
         <v>36.107963400000003</v>
       </c>
-      <c r="R21" s="9">
+      <c r="T21" s="9">
         <v>24.829212200000001</v>
       </c>
-      <c r="S21" s="9">
+      <c r="U21" s="9">
         <v>153.56662</v>
       </c>
-      <c r="T21" s="10">
+      <c r="V21" s="10">
         <v>-9.2136552300000005</v>
       </c>
-      <c r="U21" s="2" t="s">
+      <c r="W21" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V21" s="2" t="s">
+      <c r="X21" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="ALB21"/>
-      <c r="ALC21"/>
       <c r="ALD21"/>
       <c r="ALE21"/>
       <c r="ALF21"/>
@@ -2745,8 +2917,10 @@
       <c r="AMH21"/>
       <c r="AMI21"/>
       <c r="AMJ21"/>
+      <c r="AMK21"/>
+      <c r="AML21"/>
     </row>
-    <row r="22" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>1255</v>
       </c>
@@ -2763,56 +2937,62 @@
         <v>0.944367821169244</v>
       </c>
       <c r="F22" s="2">
+        <f t="shared" si="0"/>
+        <v>0.24802147890646248</v>
+      </c>
+      <c r="G22" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.63032353788807005</v>
+      </c>
+      <c r="H22" s="2">
         <v>-5.1292627013548697E-2</v>
       </c>
-      <c r="G22" s="2">
+      <c r="I22" s="2">
         <v>0.62920605222520898</v>
       </c>
-      <c r="H22" s="2">
+      <c r="J22" s="2">
         <v>-0.54347826086956597</v>
       </c>
-      <c r="I22" s="2">
+      <c r="K22" s="2">
         <v>-7.9092627599243901</v>
       </c>
-      <c r="J22" s="2">
+      <c r="L22" s="2">
         <v>0.30787462863475901</v>
       </c>
-      <c r="K22" s="2">
+      <c r="M22" s="2">
         <v>-0.65707965357793496</v>
       </c>
-      <c r="L22" s="5">
+      <c r="N22" s="5">
         <v>0.621326051957662</v>
       </c>
-      <c r="M22" s="1"/>
-      <c r="N22">
+      <c r="O22" s="1"/>
+      <c r="P22">
         <v>34.020102899999998</v>
       </c>
-      <c r="O22">
+      <c r="Q22">
         <v>48.960192599999999</v>
       </c>
-      <c r="P22" s="9">
+      <c r="R22" s="9">
         <v>-65.344363999999999</v>
       </c>
-      <c r="Q22" s="9">
+      <c r="S22" s="9">
         <v>12.029044600000001</v>
       </c>
-      <c r="R22" s="9">
+      <c r="T22" s="9">
         <v>58.6439819</v>
       </c>
-      <c r="S22" s="9">
+      <c r="U22" s="9">
         <v>74.448393199999998</v>
       </c>
-      <c r="T22" s="10">
+      <c r="V22" s="10">
         <v>-1.89919949</v>
       </c>
-      <c r="U22" s="2" t="s">
+      <c r="W22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V22" s="2" t="s">
+      <c r="X22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="ALB22"/>
-      <c r="ALC22"/>
       <c r="ALD22"/>
       <c r="ALE22"/>
       <c r="ALF22"/>
@@ -2846,8 +3026,10 @@
       <c r="AMH22"/>
       <c r="AMI22"/>
       <c r="AMJ22"/>
+      <c r="AMK22"/>
+      <c r="AML22"/>
     </row>
-    <row r="23" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>3189</v>
       </c>
@@ -2864,56 +3046,62 @@
         <v>0.57533326533559803</v>
       </c>
       <c r="F23" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.12523453605076895</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" si="1"/>
+        <v>-2.3210954391670979E-2</v>
+      </c>
+      <c r="H23" s="2">
         <v>-0.64577699217615803</v>
       </c>
-      <c r="G23" s="2">
+      <c r="I23" s="2">
         <v>0.56372778813976299</v>
       </c>
-      <c r="H23" s="2">
+      <c r="J23" s="2">
         <v>-0.54347826086956597</v>
       </c>
-      <c r="I23" s="2">
+      <c r="K23" s="2">
         <v>-7.9092627599243901</v>
       </c>
-      <c r="J23" s="2">
+      <c r="L23" s="2">
         <v>0.37005101651759797</v>
       </c>
-      <c r="K23" s="2">
+      <c r="M23" s="2">
         <v>-0.690871168731652</v>
       </c>
-      <c r="L23" s="5">
+      <c r="N23" s="5">
         <v>0.12955666272931099</v>
       </c>
-      <c r="M23" s="1"/>
-      <c r="N23">
+      <c r="O23" s="1"/>
+      <c r="P23">
         <v>25.465853589999998</v>
       </c>
-      <c r="O23">
+      <c r="Q23">
         <v>-42.647148860000001</v>
       </c>
-      <c r="P23" s="9">
+      <c r="R23" s="9">
         <v>40.314688599999997</v>
       </c>
-      <c r="Q23" s="9">
+      <c r="S23" s="9">
         <v>75.293011300000003</v>
       </c>
-      <c r="R23" s="9">
+      <c r="T23" s="9">
         <v>52.198349</v>
       </c>
-      <c r="S23" s="9">
+      <c r="U23" s="9">
         <v>27.431182199999999</v>
       </c>
-      <c r="T23" s="10">
+      <c r="V23" s="10">
         <v>-21.740797499999999</v>
       </c>
-      <c r="U23" s="2" t="s">
+      <c r="W23" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V23" s="2" t="s">
+      <c r="X23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="ALB23"/>
-      <c r="ALC23"/>
       <c r="ALD23"/>
       <c r="ALE23"/>
       <c r="ALF23"/>
@@ -2947,8 +3135,10 @@
       <c r="AMH23"/>
       <c r="AMI23"/>
       <c r="AMJ23"/>
+      <c r="AMK23"/>
+      <c r="AML23"/>
     </row>
-    <row r="24" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>3206</v>
       </c>
@@ -2965,56 +3155,62 @@
         <v>-0.135090093012217</v>
       </c>
       <c r="F24" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.10974395186385799</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="1"/>
+        <v>0.48126121229290897</v>
+      </c>
+      <c r="H24" s="2">
         <v>-0.64986147944520301</v>
       </c>
-      <c r="G24" s="2">
+      <c r="I24" s="2">
         <v>0.105540513134238</v>
       </c>
-      <c r="H24" s="2">
+      <c r="J24" s="2">
         <v>-0.54347826086956597</v>
       </c>
-      <c r="I24" s="2">
+      <c r="K24" s="2">
         <v>-7.9092627599243901</v>
       </c>
-      <c r="J24" s="2">
+      <c r="L24" s="2">
         <v>2.2474921985822198</v>
       </c>
-      <c r="K24" s="2">
+      <c r="M24" s="2">
         <v>-1.7112196372450299</v>
       </c>
-      <c r="L24" s="5">
+      <c r="N24" s="5">
         <v>-14.7196189625228</v>
       </c>
-      <c r="M24" s="1"/>
-      <c r="N24">
+      <c r="O24" s="1"/>
+      <c r="P24">
         <v>-17.74076835</v>
       </c>
-      <c r="O24">
+      <c r="Q24">
         <v>50.625313949999999</v>
       </c>
-      <c r="P24" s="9">
+      <c r="R24" s="9">
         <v>18.8679378</v>
       </c>
-      <c r="Q24" s="9">
+      <c r="S24" s="9">
         <v>-34.455466999999999</v>
       </c>
-      <c r="R24" s="9">
+      <c r="T24" s="9">
         <v>-5.7978095999999999</v>
       </c>
-      <c r="S24" s="9">
+      <c r="U24" s="9">
         <v>48.281009699999998</v>
       </c>
-      <c r="T24" s="10">
+      <c r="V24" s="10">
         <v>-26.221789399999999</v>
       </c>
-      <c r="U24" s="2" t="s">
+      <c r="W24" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V24" s="2" t="s">
+      <c r="X24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="ALB24"/>
-      <c r="ALC24"/>
       <c r="ALD24"/>
       <c r="ALE24"/>
       <c r="ALF24"/>
@@ -3048,8 +3244,10 @@
       <c r="AMH24"/>
       <c r="AMI24"/>
       <c r="AMJ24"/>
+      <c r="AMK24"/>
+      <c r="AML24"/>
     </row>
-    <row r="25" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>1001</v>
       </c>
@@ -3066,56 +3264,62 @@
         <v>-1.4300900821315199</v>
       </c>
       <c r="F25" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15340385065409212</v>
+      </c>
+      <c r="G25" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.60205028700197016</v>
+      </c>
+      <c r="H25" s="2">
         <v>1.0278050104788801</v>
       </c>
-      <c r="G25" s="2">
+      <c r="I25" s="2">
         <v>-1.73111522563251</v>
       </c>
-      <c r="H25" s="2">
+      <c r="J25" s="2">
         <v>0.45652173913043498</v>
       </c>
-      <c r="I25" s="2">
+      <c r="K25" s="2">
         <v>-7.99621928166352</v>
       </c>
-      <c r="J25" s="2">
+      <c r="L25" s="2">
         <v>0.500729969459494</v>
       </c>
-      <c r="K25" s="2">
+      <c r="M25" s="2">
         <v>-0.261162369349275</v>
       </c>
-      <c r="L25" s="5">
+      <c r="N25" s="5">
         <v>-0.94755924975467698</v>
       </c>
-      <c r="M25" s="1"/>
-      <c r="N25">
+      <c r="O25" s="1"/>
+      <c r="P25">
         <v>104.44815509999999</v>
       </c>
-      <c r="O25">
+      <c r="Q25">
         <v>-39.978097750000003</v>
       </c>
-      <c r="P25" s="9">
+      <c r="R25" s="9">
         <v>38.503434400000003</v>
       </c>
-      <c r="Q25" s="9">
+      <c r="S25" s="9">
         <v>-13.475479999999999</v>
       </c>
-      <c r="R25" s="9">
+      <c r="T25" s="9">
         <v>55.680831900000001</v>
       </c>
-      <c r="S25" s="9">
+      <c r="U25" s="9">
         <v>146.49041399999999</v>
       </c>
-      <c r="T25" s="10">
+      <c r="V25" s="10">
         <v>-4.8224854500000003</v>
       </c>
-      <c r="U25" s="2" t="s">
+      <c r="W25" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V25" s="2" t="s">
+      <c r="X25" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="ALB25"/>
-      <c r="ALC25"/>
       <c r="ALD25"/>
       <c r="ALE25"/>
       <c r="ALF25"/>
@@ -3149,8 +3353,10 @@
       <c r="AMH25"/>
       <c r="AMI25"/>
       <c r="AMJ25"/>
+      <c r="AMK25"/>
+      <c r="AML25"/>
     </row>
-    <row r="26" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>1286</v>
       </c>
@@ -3167,56 +3373,62 @@
         <v>-0.23377752271603999</v>
       </c>
       <c r="F26" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.21929258508823002</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.22358401534764602</v>
+      </c>
+      <c r="H26" s="2">
         <v>-0.79557934548294795</v>
       </c>
-      <c r="G26" s="2">
+      <c r="I26" s="2">
         <v>-0.34556953038986299</v>
       </c>
-      <c r="H26" s="2">
+      <c r="J26" s="2">
         <v>0.45652173913043498</v>
       </c>
-      <c r="I26" s="2">
+      <c r="K26" s="2">
         <v>-7.99621928166352</v>
       </c>
-      <c r="J26" s="2">
+      <c r="L26" s="2">
         <v>-0.84925741573508895</v>
       </c>
-      <c r="K26" s="2">
+      <c r="M26" s="2">
         <v>-0.87746095824245396</v>
       </c>
-      <c r="L26" s="5">
+      <c r="N26" s="5">
         <v>9.8472359097407605</v>
       </c>
-      <c r="M26" s="1"/>
-      <c r="N26">
+      <c r="O26" s="1"/>
+      <c r="P26">
         <v>30.1115259</v>
       </c>
-      <c r="O26">
+      <c r="Q26">
         <v>49.45746879</v>
       </c>
-      <c r="P26" s="9">
+      <c r="R26" s="9">
         <v>4.3254374599999998</v>
       </c>
-      <c r="Q26" s="9">
+      <c r="S26" s="9">
         <v>-13.301997999999999</v>
       </c>
-      <c r="R26" s="9">
+      <c r="T26" s="9">
         <v>-33.464962</v>
       </c>
-      <c r="S26" s="9">
+      <c r="U26" s="9">
         <v>28.920974099999999</v>
       </c>
-      <c r="T26" s="10">
+      <c r="V26" s="10">
         <v>-5.1670048199999998</v>
       </c>
-      <c r="U26" s="2" t="s">
+      <c r="W26" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V26" s="2" t="s">
+      <c r="X26" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="ALB26"/>
-      <c r="ALC26"/>
       <c r="ALD26"/>
       <c r="ALE26"/>
       <c r="ALF26"/>
@@ -3250,8 +3462,10 @@
       <c r="AMH26"/>
       <c r="AMI26"/>
       <c r="AMJ26"/>
+      <c r="AMK26"/>
+      <c r="AML26"/>
     </row>
-    <row r="27" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>1303</v>
       </c>
@@ -3268,56 +3482,62 @@
         <v>-1.69682879227923</v>
       </c>
       <c r="F27" s="2">
+        <f t="shared" si="0"/>
+        <v>-2.1452670731491097E-2</v>
+      </c>
+      <c r="G27" s="2">
+        <f t="shared" si="1"/>
+        <v>9.7395930373729955E-2</v>
+      </c>
+      <c r="H27" s="2">
         <v>-8.0986892580062406E-2</v>
       </c>
-      <c r="G27" s="2">
+      <c r="I27" s="2">
         <v>-1.64813082709236</v>
       </c>
-      <c r="H27" s="2">
+      <c r="J27" s="2">
         <v>0.45652173913043498</v>
       </c>
-      <c r="I27" s="2">
+      <c r="K27" s="2">
         <v>-7.99621928166352</v>
       </c>
-      <c r="J27" s="2">
+      <c r="L27" s="2">
         <v>3.0473680641410601</v>
       </c>
-      <c r="K27" s="2">
+      <c r="M27" s="2">
         <v>0.90143328257056998</v>
       </c>
-      <c r="L27" s="5">
+      <c r="N27" s="5">
         <v>-21.3110358858663</v>
       </c>
-      <c r="M27" s="1"/>
-      <c r="N27">
+      <c r="O27" s="1"/>
+      <c r="P27">
         <v>35.635082650000001</v>
       </c>
-      <c r="O27">
+      <c r="Q27">
         <v>33.704344229999997</v>
       </c>
-      <c r="P27" s="9">
+      <c r="R27" s="9">
         <v>63.181349699999998</v>
       </c>
-      <c r="Q27" s="9">
+      <c r="S27" s="9">
         <v>-10.609337999999999</v>
       </c>
-      <c r="R27" s="9">
+      <c r="T27" s="9">
         <v>51.451114699999998</v>
       </c>
-      <c r="S27" s="9">
+      <c r="U27" s="9">
         <v>54.760132499999997</v>
       </c>
-      <c r="T27" s="10">
+      <c r="V27" s="10">
         <v>16.345963999999999</v>
       </c>
-      <c r="U27" s="2" t="s">
+      <c r="W27" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V27" s="2" t="s">
+      <c r="X27" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="ALB27"/>
-      <c r="ALC27"/>
       <c r="ALD27"/>
       <c r="ALE27"/>
       <c r="ALF27"/>
@@ -3351,8 +3571,10 @@
       <c r="AMH27"/>
       <c r="AMI27"/>
       <c r="AMJ27"/>
+      <c r="AMK27"/>
+      <c r="AML27"/>
     </row>
-    <row r="28" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>3143</v>
       </c>
@@ -3369,56 +3591,62 @@
         <v>0.40193846279968898</v>
       </c>
       <c r="F28" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0302816771233019</v>
+      </c>
+      <c r="G28" s="2">
+        <f t="shared" si="1"/>
+        <v>-2.2581105720930492</v>
+      </c>
+      <c r="H28" s="2">
         <v>-0.58704243912773901</v>
       </c>
-      <c r="G28" s="2">
+      <c r="I28" s="2">
         <v>-0.72711682324683502</v>
       </c>
-      <c r="H28" s="2">
+      <c r="J28" s="2">
         <v>0.45652173913043498</v>
       </c>
-      <c r="I28" s="2">
+      <c r="K28" s="2">
         <v>-7.99621928166352</v>
       </c>
-      <c r="J28" s="2">
+      <c r="L28" s="2">
         <v>7.1363194863161103</v>
       </c>
-      <c r="K28" s="2">
+      <c r="M28" s="2">
         <v>2.7681284970417899</v>
       </c>
-      <c r="L28" s="5">
+      <c r="N28" s="5">
         <v>-54.007188089647798</v>
       </c>
-      <c r="M28" s="1"/>
-      <c r="N28">
+      <c r="O28" s="1"/>
+      <c r="P28">
         <v>-2.0525630769999998</v>
       </c>
-      <c r="O28">
+      <c r="Q28">
         <v>-17.27218384</v>
       </c>
-      <c r="P28" s="9">
+      <c r="R28" s="9">
         <v>-1.9140714000000001</v>
       </c>
-      <c r="Q28" s="9">
+      <c r="S28" s="9">
         <v>-13.370723999999999</v>
       </c>
-      <c r="R28" s="9">
+      <c r="T28" s="9">
         <v>-16.247821999999999</v>
       </c>
-      <c r="S28" s="9">
+      <c r="U28" s="9">
         <v>-8.7662104000000003</v>
       </c>
-      <c r="T28" s="10">
+      <c r="V28" s="10">
         <v>-3.0872554800000001</v>
       </c>
-      <c r="U28" s="2" t="s">
+      <c r="W28" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V28" s="2" t="s">
+      <c r="X28" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="ALB28"/>
-      <c r="ALC28"/>
       <c r="ALD28"/>
       <c r="ALE28"/>
       <c r="ALF28"/>
@@ -3452,8 +3680,10 @@
       <c r="AMH28"/>
       <c r="AMI28"/>
       <c r="AMJ28"/>
+      <c r="AMK28"/>
+      <c r="AML28"/>
     </row>
-    <row r="29" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>1009</v>
       </c>
@@ -3470,56 +3700,62 @@
         <v>0.43316364971270299</v>
       </c>
       <c r="F29" s="2">
+        <f t="shared" si="0"/>
+        <v>0.12533966851417039</v>
+      </c>
+      <c r="G29" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.36164469318746328</v>
+      </c>
+      <c r="H29" s="2">
         <v>1.2885473647255501E-2</v>
       </c>
-      <c r="G29" s="2">
+      <c r="I29" s="2">
         <v>0.25234130311897102</v>
       </c>
-      <c r="H29" s="2">
+      <c r="J29" s="2">
         <v>1.4565217391304299</v>
       </c>
-      <c r="I29" s="2">
+      <c r="K29" s="2">
         <v>-6.08317580340265</v>
       </c>
-      <c r="J29" s="2">
+      <c r="L29" s="2">
         <v>-1.1385404268275501</v>
       </c>
-      <c r="K29" s="2">
+      <c r="M29" s="2">
         <v>-2.1480653683948199</v>
       </c>
-      <c r="L29" s="5">
+      <c r="N29" s="5">
         <v>9.9823289626171903</v>
       </c>
-      <c r="M29" s="1"/>
-      <c r="N29">
+      <c r="O29" s="1"/>
+      <c r="P29">
         <v>2.494506474</v>
       </c>
-      <c r="O29">
+      <c r="Q29">
         <v>38.770238740000003</v>
       </c>
-      <c r="P29" s="9">
+      <c r="R29" s="9">
         <v>-6.4283463999999997</v>
       </c>
-      <c r="Q29" s="9">
+      <c r="S29" s="9">
         <v>-86.326468000000006</v>
       </c>
-      <c r="R29" s="9">
+      <c r="T29" s="9">
         <v>20.4448471</v>
       </c>
-      <c r="S29" s="9">
+      <c r="U29" s="9">
         <v>20.850715000000001</v>
       </c>
-      <c r="T29" s="10">
+      <c r="V29" s="10">
         <v>16.786358799999999</v>
       </c>
-      <c r="U29" s="2" t="s">
+      <c r="W29" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V29" s="2" t="s">
+      <c r="X29" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="ALB29"/>
-      <c r="ALC29"/>
       <c r="ALD29"/>
       <c r="ALE29"/>
       <c r="ALF29"/>
@@ -3553,8 +3789,10 @@
       <c r="AMH29"/>
       <c r="AMI29"/>
       <c r="AMJ29"/>
+      <c r="AMK29"/>
+      <c r="AML29"/>
     </row>
-    <row r="30" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>1249</v>
       </c>
@@ -3571,56 +3809,62 @@
         <v>0.88447901557917796</v>
       </c>
       <c r="F30" s="2">
+        <f t="shared" si="0"/>
+        <v>-3.0513280469032025E-3</v>
+      </c>
+      <c r="G30" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.32359872137326295</v>
+      </c>
+      <c r="H30" s="2">
         <v>-4.8533200467733698E-2</v>
       </c>
-      <c r="G30" s="2">
+      <c r="I30" s="2">
         <v>0.72267965489254604</v>
       </c>
-      <c r="H30" s="2">
+      <c r="J30" s="2">
         <v>1.4565217391304299</v>
       </c>
-      <c r="I30" s="2">
+      <c r="K30" s="2">
         <v>-6.08317580340265</v>
       </c>
-      <c r="J30" s="2">
+      <c r="L30" s="2">
         <v>8.6564785260837801E-2</v>
       </c>
-      <c r="K30" s="2">
+      <c r="M30" s="2">
         <v>-0.36367299426608501</v>
       </c>
-      <c r="L30" s="5">
+      <c r="N30" s="5">
         <v>2.5297985798186402</v>
       </c>
-      <c r="M30" s="1"/>
-      <c r="N30">
+      <c r="O30" s="1"/>
+      <c r="P30">
         <v>22.743217510000001</v>
       </c>
-      <c r="O30">
+      <c r="Q30">
         <v>5.3051316379999998</v>
       </c>
-      <c r="P30" s="9">
+      <c r="R30" s="9">
         <v>-44.668028</v>
       </c>
-      <c r="Q30" s="9">
+      <c r="S30" s="9">
         <v>46.017015899999997</v>
       </c>
-      <c r="R30" s="9">
+      <c r="T30" s="9">
         <v>-11.481002999999999</v>
       </c>
-      <c r="S30" s="9">
+      <c r="U30" s="9">
         <v>29.661425300000001</v>
       </c>
-      <c r="T30" s="10">
+      <c r="V30" s="10">
         <v>-9.6917865299999999</v>
       </c>
-      <c r="U30" s="2" t="s">
+      <c r="W30" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V30" s="2" t="s">
+      <c r="X30" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="ALB30"/>
-      <c r="ALC30"/>
       <c r="ALD30"/>
       <c r="ALE30"/>
       <c r="ALF30"/>
@@ -3654,8 +3898,10 @@
       <c r="AMH30"/>
       <c r="AMI30"/>
       <c r="AMJ30"/>
+      <c r="AMK30"/>
+      <c r="AML30"/>
     </row>
-    <row r="31" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>3116</v>
       </c>
@@ -3672,56 +3918,62 @@
         <v>-0.87084719935352595</v>
       </c>
       <c r="F31" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.66680438651980711</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" si="1"/>
+        <v>1.6431329271569628</v>
+      </c>
+      <c r="H31" s="2">
         <v>0.73332302172963704</v>
       </c>
-      <c r="G31" s="2">
+      <c r="I31" s="2">
         <v>-4.92807357750445E-2</v>
       </c>
-      <c r="H31" s="2">
+      <c r="J31" s="2">
         <v>1.4565217391304299</v>
       </c>
-      <c r="I31" s="2">
+      <c r="K31" s="2">
         <v>-6.08317580340265</v>
       </c>
-      <c r="J31" s="2">
+      <c r="L31" s="2">
         <v>-0.84925741573508895</v>
       </c>
-      <c r="K31" s="2">
+      <c r="M31" s="2">
         <v>-1.72671837397754</v>
       </c>
-      <c r="L31" s="5">
+      <c r="N31" s="5">
         <v>8.2225695492040707</v>
       </c>
-      <c r="M31" s="1"/>
-      <c r="N31">
+      <c r="O31" s="1"/>
+      <c r="P31">
         <v>-10.87655007</v>
       </c>
-      <c r="O31">
+      <c r="Q31">
         <v>-2.5690697899999999</v>
       </c>
-      <c r="P31" s="9">
+      <c r="R31" s="9">
         <v>46.590738000000002</v>
       </c>
-      <c r="Q31" s="9">
+      <c r="S31" s="9">
         <v>-93.432942999999995</v>
       </c>
-      <c r="R31" s="9">
+      <c r="T31" s="9">
         <v>-26.289515000000002</v>
       </c>
-      <c r="S31" s="9">
+      <c r="U31" s="9">
         <v>-66.270713999999998</v>
       </c>
-      <c r="T31" s="10">
+      <c r="V31" s="10">
         <v>-21.8935125</v>
       </c>
-      <c r="U31" s="2" t="s">
+      <c r="W31" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V31" s="2" t="s">
+      <c r="X31" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="ALB31"/>
-      <c r="ALC31"/>
       <c r="ALD31"/>
       <c r="ALE31"/>
       <c r="ALF31"/>
@@ -3755,8 +4007,10 @@
       <c r="AMH31"/>
       <c r="AMI31"/>
       <c r="AMJ31"/>
+      <c r="AMK31"/>
+      <c r="AML31"/>
     </row>
-    <row r="32" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>3199</v>
       </c>
@@ -3773,56 +4027,62 @@
         <v>-1.08918234478971</v>
       </c>
       <c r="F32" s="2">
+        <f t="shared" si="0"/>
+        <v>6.2707500578619957E-2</v>
+      </c>
+      <c r="G32" s="2">
+        <f t="shared" si="1"/>
+        <v>8.5020697559210046E-2</v>
+      </c>
+      <c r="H32" s="2">
         <v>1.1837366822173301</v>
       </c>
-      <c r="G32" s="2">
+      <c r="I32" s="2">
         <v>-1.0466719960101101</v>
       </c>
-      <c r="H32" s="2">
+      <c r="J32" s="2">
         <v>1.4565217391304299</v>
       </c>
-      <c r="I32" s="2">
+      <c r="K32" s="2">
         <v>-6.08317580340265</v>
       </c>
-      <c r="J32" s="2">
+      <c r="L32" s="2">
         <v>-0.55997440464262704</v>
       </c>
-      <c r="K32" s="2">
+      <c r="M32" s="2">
         <v>-1.3053713795602599</v>
       </c>
-      <c r="L32" s="5">
+      <c r="N32" s="5">
         <v>6.4628101357909404</v>
       </c>
-      <c r="M32" s="1"/>
-      <c r="N32">
+      <c r="O32" s="1"/>
+      <c r="P32">
         <v>38.044908</v>
       </c>
-      <c r="O32">
+      <c r="Q32">
         <v>86.443887129999993</v>
       </c>
-      <c r="P32" s="9">
+      <c r="R32" s="9">
         <v>-82.625489000000002</v>
       </c>
-      <c r="Q32" s="9">
+      <c r="S32" s="9">
         <v>-6.5832949999999997</v>
       </c>
-      <c r="R32" s="9">
+      <c r="T32" s="9">
         <v>108.666901</v>
       </c>
-      <c r="S32" s="9">
+      <c r="U32" s="9">
         <v>3.0840355599999998</v>
       </c>
-      <c r="T32" s="10">
+      <c r="V32" s="10">
         <v>-21.5328555</v>
       </c>
-      <c r="U32" s="2" t="s">
+      <c r="W32" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V32" s="2" t="s">
+      <c r="X32" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="ALB32"/>
-      <c r="ALC32"/>
       <c r="ALD32"/>
       <c r="ALE32"/>
       <c r="ALF32"/>
@@ -3856,8 +4116,10 @@
       <c r="AMH32"/>
       <c r="AMI32"/>
       <c r="AMJ32"/>
+      <c r="AMK32"/>
+      <c r="AML32"/>
     </row>
-    <row r="33" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="11">
         <v>3220</v>
       </c>
@@ -3873,57 +4135,63 @@
       <c r="E33" s="11">
         <v>0.45353431228712698</v>
       </c>
-      <c r="F33" s="11">
+      <c r="F33" s="2">
+        <f t="shared" si="0"/>
+        <v>0.16017006479019402</v>
+      </c>
+      <c r="G33" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.98130300467617704</v>
+      </c>
+      <c r="H33" s="11">
         <v>0.191482683050193</v>
       </c>
-      <c r="G33" s="11">
+      <c r="I33" s="11">
         <v>-3.71171900509615E-2</v>
       </c>
-      <c r="H33" s="11">
+      <c r="J33" s="11">
         <v>1.4565217391304299</v>
       </c>
-      <c r="I33" s="11">
+      <c r="K33" s="11">
         <v>-6.08317580340265</v>
       </c>
-      <c r="J33" s="11">
+      <c r="L33" s="11">
         <v>1.85916175422969E-2</v>
       </c>
-      <c r="K33" s="11">
+      <c r="M33" s="11">
         <v>-0.46267739072569902</v>
       </c>
-      <c r="L33" s="5">
+      <c r="N33" s="5">
         <v>2.9432913089646902</v>
       </c>
-      <c r="M33" s="1"/>
-      <c r="N33">
+      <c r="O33" s="1"/>
+      <c r="P33">
         <v>6.1268146100000003</v>
       </c>
-      <c r="O33">
+      <c r="Q33">
         <v>4.0158694229999998</v>
       </c>
-      <c r="P33" s="9">
+      <c r="R33" s="9">
         <v>36.241843699999997</v>
       </c>
-      <c r="Q33" s="9">
+      <c r="S33" s="9">
         <v>4.95889588</v>
       </c>
-      <c r="R33" s="9">
+      <c r="T33" s="9">
         <v>-12.92651</v>
       </c>
-      <c r="S33" s="9">
+      <c r="U33" s="9">
         <v>77.791620899999998</v>
       </c>
-      <c r="T33" s="10">
+      <c r="V33" s="10">
         <v>1.3800907099999999</v>
       </c>
-      <c r="U33" s="2" t="s">
+      <c r="W33" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V33" s="2" t="s">
+      <c r="X33" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="ALB33"/>
-      <c r="ALC33"/>
       <c r="ALD33"/>
       <c r="ALE33"/>
       <c r="ALF33"/>
@@ -3957,8 +4225,10 @@
       <c r="AMH33"/>
       <c r="AMI33"/>
       <c r="AMJ33"/>
+      <c r="AMK33"/>
+      <c r="AML33"/>
     </row>
-    <row r="34" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>1004</v>
       </c>
@@ -3975,56 +4245,62 @@
         <v>-9.87342832775015E-3</v>
       </c>
       <c r="F34" s="2">
+        <f t="shared" si="0"/>
+        <v>0.34643394561572405</v>
+      </c>
+      <c r="G34" s="2">
+        <f t="shared" si="1"/>
+        <v>-1.2554231788978998</v>
+      </c>
+      <c r="H34" s="2">
         <v>-0.487097714872817</v>
       </c>
-      <c r="G34" s="2">
+      <c r="I34" s="2">
         <v>-0.63758501777669996</v>
       </c>
-      <c r="H34" s="2">
+      <c r="J34" s="2">
         <v>2.4565217391304301</v>
       </c>
-      <c r="I34" s="2">
+      <c r="K34" s="2">
         <v>-2.1701323251417799</v>
       </c>
-      <c r="J34" s="2">
+      <c r="L34" s="2">
         <v>-0.27069139355016503</v>
       </c>
-      <c r="K34" s="2">
+      <c r="M34" s="2">
         <v>-1.1547157786931499</v>
       </c>
-      <c r="L34" s="5">
+      <c r="N34" s="5">
         <v>3.6438235302250002</v>
       </c>
-      <c r="M34" s="1"/>
-      <c r="N34">
+      <c r="O34" s="1"/>
+      <c r="P34">
         <v>-39.001481699999999</v>
       </c>
-      <c r="O34">
+      <c r="Q34">
         <v>-0.43271195109999999</v>
       </c>
-      <c r="P34" s="9">
+      <c r="R34" s="9">
         <v>10.4736101</v>
       </c>
-      <c r="Q34" s="9">
+      <c r="S34" s="9">
         <v>-24.121327999999998</v>
       </c>
-      <c r="R34" s="9">
+      <c r="T34" s="9">
         <v>32.432022099999998</v>
       </c>
-      <c r="S34" s="9">
+      <c r="U34" s="9">
         <v>-28.917687000000001</v>
       </c>
-      <c r="T34" s="10">
+      <c r="V34" s="10">
         <v>-7.2744746200000003</v>
       </c>
-      <c r="U34" s="2" t="s">
+      <c r="W34" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V34" s="2" t="s">
+      <c r="X34" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="ALB34"/>
-      <c r="ALC34"/>
       <c r="ALD34"/>
       <c r="ALE34"/>
       <c r="ALF34"/>
@@ -4058,8 +4334,10 @@
       <c r="AMH34"/>
       <c r="AMI34"/>
       <c r="AMJ34"/>
+      <c r="AMK34"/>
+      <c r="AML34"/>
     </row>
-    <row r="35" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>1019</v>
       </c>
@@ -4076,56 +4354,62 @@
         <v>-1.196642174415</v>
       </c>
       <c r="F35" s="2">
+        <f t="shared" si="0"/>
+        <v>0.43685911634570934</v>
+      </c>
+      <c r="G35" s="2">
+        <f t="shared" si="1"/>
+        <v>0.10368429823608993</v>
+      </c>
+      <c r="H35" s="2">
         <v>0.283292637963522</v>
       </c>
-      <c r="G35" s="2">
+      <c r="I35" s="2">
         <v>-1.1448000252969599</v>
       </c>
-      <c r="H35" s="2">
+      <c r="J35" s="2">
         <v>2.4565217391304301</v>
       </c>
-      <c r="I35" s="2">
+      <c r="K35" s="2">
         <v>-2.1701323251417799</v>
       </c>
-      <c r="J35" s="2">
+      <c r="L35" s="2">
         <v>1.85916175422969E-2</v>
       </c>
-      <c r="K35" s="2">
+      <c r="M35" s="2">
         <v>-0.44408577318340198</v>
       </c>
-      <c r="L35" s="5">
+      <c r="N35" s="5">
         <v>3.0160411167388999</v>
       </c>
-      <c r="M35" s="1"/>
-      <c r="N35">
+      <c r="O35" s="1"/>
+      <c r="P35">
         <v>-32.559631869999997</v>
       </c>
-      <c r="O35">
+      <c r="Q35">
         <v>25.00740184</v>
       </c>
-      <c r="P35" s="9">
+      <c r="R35" s="9">
         <v>-20.744482999999999</v>
       </c>
-      <c r="Q35" s="9">
+      <c r="S35" s="9">
         <v>-42.182209999999998</v>
       </c>
-      <c r="R35" s="9">
+      <c r="T35" s="9">
         <v>-34.189720000000001</v>
       </c>
-      <c r="S35" s="9">
+      <c r="U35" s="9">
         <v>54.625435400000001</v>
       </c>
-      <c r="T35" s="10">
+      <c r="V35" s="10">
         <v>-18.1640902</v>
       </c>
-      <c r="U35" s="2" t="s">
+      <c r="W35" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V35" s="2" t="s">
+      <c r="X35" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="ALB35"/>
-      <c r="ALC35"/>
       <c r="ALD35"/>
       <c r="ALE35"/>
       <c r="ALF35"/>
@@ -4159,8 +4443,10 @@
       <c r="AMH35"/>
       <c r="AMI35"/>
       <c r="AMJ35"/>
+      <c r="AMK35"/>
+      <c r="AML35"/>
     </row>
-    <row r="36" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>1242</v>
       </c>
@@ -4177,56 +4463,62 @@
         <v>1.2424218404799099</v>
       </c>
       <c r="F36" s="2">
+        <f t="shared" si="0"/>
+        <v>4.0913493217239916E-2</v>
+      </c>
+      <c r="G36" s="2">
+        <f t="shared" si="1"/>
+        <v>1.5444809097160173E-2</v>
+      </c>
+      <c r="H36" s="2">
         <v>-1.3576318132741301</v>
       </c>
-      <c r="G36" s="2">
+      <c r="I36" s="2">
         <v>1.2501442450284901</v>
       </c>
-      <c r="H36" s="2">
+      <c r="J36" s="2">
         <v>2.4565217391304301</v>
       </c>
-      <c r="I36" s="2">
+      <c r="K36" s="2">
         <v>-2.1701323251417799</v>
       </c>
-      <c r="J36" s="2">
+      <c r="L36" s="2">
         <v>1.4650066730046101</v>
       </c>
-      <c r="K36" s="2">
+      <c r="M36" s="2">
         <v>3.10906425436532</v>
       </c>
-      <c r="L36" s="5">
+      <c r="N36" s="5">
         <v>-0.122870950691603</v>
       </c>
-      <c r="M36" s="1"/>
-      <c r="N36">
+      <c r="O36" s="1"/>
+      <c r="P36">
         <v>-29.55395721</v>
       </c>
-      <c r="O36">
+      <c r="Q36">
         <v>-15.142114680000001</v>
       </c>
-      <c r="P36" s="9">
+      <c r="R36" s="9">
         <v>-1.6757515000000001</v>
       </c>
-      <c r="Q36" s="9">
+      <c r="S36" s="9">
         <v>-52.677019000000001</v>
       </c>
-      <c r="R36" s="9">
+      <c r="T36" s="9">
         <v>-54.459502999999998</v>
       </c>
-      <c r="S36" s="9">
+      <c r="U36" s="9">
         <v>12.1930508</v>
       </c>
-      <c r="T36" s="10">
+      <c r="V36" s="10">
         <v>-3.6567214699999999</v>
       </c>
-      <c r="U36" s="2" t="s">
+      <c r="W36" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V36" s="2" t="s">
+      <c r="X36" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="ALB36"/>
-      <c r="ALC36"/>
       <c r="ALD36"/>
       <c r="ALE36"/>
       <c r="ALF36"/>
@@ -4260,8 +4552,10 @@
       <c r="AMH36"/>
       <c r="AMI36"/>
       <c r="AMJ36"/>
+      <c r="AMK36"/>
+      <c r="AML36"/>
     </row>
-    <row r="37" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>1247</v>
       </c>
@@ -4278,56 +4572,62 @@
         <v>4.8497383402055699E-2</v>
       </c>
       <c r="F37" s="2">
+        <f t="shared" si="0"/>
+        <v>0.13252339886286801</v>
+      </c>
+      <c r="G37" s="2">
+        <f t="shared" si="1"/>
+        <v>0.33323572079259134</v>
+      </c>
+      <c r="H37" s="2">
         <v>0.89736618888804498</v>
       </c>
-      <c r="G37" s="2">
+      <c r="I37" s="2">
         <v>0.21511524379835101</v>
       </c>
-      <c r="H37" s="2">
+      <c r="J37" s="2">
         <v>2.4565217391304301</v>
       </c>
-      <c r="I37" s="2">
+      <c r="K37" s="2">
         <v>-2.1701323251417799</v>
       </c>
-      <c r="J37" s="2">
+      <c r="L37" s="2">
         <v>-0.55997440464262704</v>
       </c>
-      <c r="K37" s="2">
+      <c r="M37" s="2">
         <v>-1.86534578420289</v>
       </c>
-      <c r="L37" s="5">
+      <c r="N37" s="5">
         <v>4.2716059437110996</v>
       </c>
-      <c r="M37" s="1"/>
-      <c r="N37">
+      <c r="O37" s="1"/>
+      <c r="P37">
         <v>11.71056053</v>
       </c>
-      <c r="O37">
+      <c r="Q37">
         <v>-9.2690660359999999</v>
       </c>
-      <c r="P37" s="9">
+      <c r="R37" s="9">
         <v>18.243709299999999</v>
       </c>
-      <c r="Q37" s="9">
+      <c r="S37" s="9">
         <v>-7.7070542</v>
       </c>
-      <c r="R37" s="9">
+      <c r="T37" s="9">
         <v>-3.2709765000000002</v>
       </c>
-      <c r="S37" s="9">
+      <c r="U37" s="9">
         <v>-19.080860999999999</v>
       </c>
-      <c r="T37" s="10">
+      <c r="V37" s="10">
         <v>2.5315623299999999</v>
       </c>
-      <c r="U37" s="2" t="s">
+      <c r="W37" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V37" s="2" t="s">
+      <c r="X37" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="ALB37"/>
-      <c r="ALC37"/>
       <c r="ALD37"/>
       <c r="ALE37"/>
       <c r="ALF37"/>
@@ -4361,8 +4661,10 @@
       <c r="AMH37"/>
       <c r="AMI37"/>
       <c r="AMJ37"/>
+      <c r="AMK37"/>
+      <c r="AML37"/>
     </row>
-    <row r="38" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>1248</v>
       </c>
@@ -4379,56 +4681,62 @@
         <v>1.3960926123931601</v>
       </c>
       <c r="F38" s="2">
+        <f t="shared" si="0"/>
+        <v>1.5023197445112046E-2</v>
+      </c>
+      <c r="G38" s="2">
+        <f t="shared" si="1"/>
+        <v>-1.7943258896643801</v>
+      </c>
+      <c r="H38" s="2">
         <v>-0.54051944700235099</v>
       </c>
-      <c r="G38" s="2">
+      <c r="I38" s="2">
         <v>0.49892966756097001</v>
       </c>
-      <c r="H38" s="2">
+      <c r="J38" s="2">
         <v>2.4565217391304301</v>
       </c>
-      <c r="I38" s="2">
+      <c r="K38" s="2">
         <v>-2.1701323251417799</v>
       </c>
-      <c r="J38" s="2">
+      <c r="L38" s="2">
         <v>-1.4278234379200101</v>
       </c>
-      <c r="K38" s="2">
+      <c r="M38" s="2">
         <v>-3.9972358007321098</v>
       </c>
-      <c r="L38" s="5">
+      <c r="N38" s="5">
         <v>6.1549531841693899</v>
       </c>
-      <c r="M38" s="1"/>
-      <c r="N38">
+      <c r="O38" s="1"/>
+      <c r="P38">
         <v>18.935483290000001</v>
       </c>
-      <c r="O38">
+      <c r="Q38">
         <v>-24.186613879999999</v>
       </c>
-      <c r="P38" s="9">
+      <c r="R38" s="9">
         <v>20.920466900000001</v>
       </c>
-      <c r="Q38" s="9">
+      <c r="S38" s="9">
         <v>-19.400817</v>
       </c>
-      <c r="R38" s="9">
+      <c r="T38" s="9">
         <v>6.9297866800000003</v>
       </c>
-      <c r="S38" s="9">
+      <c r="U38" s="9">
         <v>51.871139100000001</v>
       </c>
-      <c r="T38" s="10">
+      <c r="V38" s="10">
         <v>-4.78914654</v>
       </c>
-      <c r="U38" s="2" t="s">
+      <c r="W38" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V38" s="2" t="s">
+      <c r="X38" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="ALB38"/>
-      <c r="ALC38"/>
       <c r="ALD38"/>
       <c r="ALE38"/>
       <c r="ALF38"/>
@@ -4462,8 +4770,10 @@
       <c r="AMH38"/>
       <c r="AMI38"/>
       <c r="AMJ38"/>
+      <c r="AMK38"/>
+      <c r="AML38"/>
     </row>
-    <row r="39" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>1016</v>
       </c>
@@ -4480,56 +4790,62 @@
         <v>1.7095233237052601</v>
       </c>
       <c r="F39" s="2">
+        <f t="shared" si="0"/>
+        <v>6.7687466931057094E-2</v>
+      </c>
+      <c r="G39" s="2">
+        <f t="shared" si="1"/>
+        <v>2.1639441919189872E-2</v>
+      </c>
+      <c r="H39" s="2">
         <v>-0.96166913445517099</v>
       </c>
-      <c r="G39" s="2">
+      <c r="I39" s="2">
         <v>1.72034304466485</v>
       </c>
-      <c r="H39" s="2">
+      <c r="J39" s="2">
         <v>3.4565217391304301</v>
       </c>
-      <c r="I39" s="2">
+      <c r="K39" s="2">
         <v>3.7429111531190902</v>
       </c>
-      <c r="J39" s="2">
+      <c r="L39" s="2">
         <v>-1.1385404268275501</v>
       </c>
-      <c r="K39" s="2">
+      <c r="M39" s="2">
         <v>-4.4251462220499196</v>
       </c>
-      <c r="L39" s="5">
+      <c r="N39" s="5">
         <v>-1.2050682749057</v>
       </c>
-      <c r="M39" s="1"/>
-      <c r="N39">
+      <c r="O39" s="1"/>
+      <c r="P39">
         <v>20.234945719999999</v>
       </c>
-      <c r="O39">
+      <c r="Q39">
         <v>24.458773480000001</v>
       </c>
-      <c r="P39" s="9">
+      <c r="R39" s="9">
         <v>7.9480848799999997</v>
       </c>
-      <c r="Q39" s="9">
+      <c r="S39" s="9">
         <v>-6.1042287000000002</v>
       </c>
-      <c r="R39" s="9">
+      <c r="T39" s="9">
         <v>55.617233300000002</v>
       </c>
-      <c r="S39" s="9">
+      <c r="U39" s="9">
         <v>-33.822575999999998</v>
       </c>
-      <c r="T39" s="10">
+      <c r="V39" s="10">
         <v>2.7318754200000002</v>
       </c>
-      <c r="U39" s="2" t="s">
+      <c r="W39" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V39" s="2" t="s">
+      <c r="X39" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="ALB39"/>
-      <c r="ALC39"/>
       <c r="ALD39"/>
       <c r="ALE39"/>
       <c r="ALF39"/>
@@ -4563,8 +4879,10 @@
       <c r="AMH39"/>
       <c r="AMI39"/>
       <c r="AMJ39"/>
+      <c r="AMK39"/>
+      <c r="AML39"/>
     </row>
-    <row r="40" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>3122</v>
       </c>
@@ -4581,56 +4899,62 @@
         <v>-0.809094967156057</v>
       </c>
       <c r="F40" s="2">
+        <f t="shared" si="0"/>
+        <v>0.38206873990802304</v>
+      </c>
+      <c r="G40" s="2">
+        <f t="shared" si="1"/>
+        <v>-9.4328078111081015E-2</v>
+      </c>
+      <c r="H40" s="2">
         <v>-0.36615969808376703</v>
       </c>
-      <c r="G40" s="2">
+      <c r="I40" s="2">
         <v>-0.85625900621159801</v>
       </c>
-      <c r="H40" s="2">
+      <c r="J40" s="2">
         <v>3.4565217391304301</v>
       </c>
-      <c r="I40" s="2">
+      <c r="K40" s="2">
         <v>3.7429111531190902</v>
       </c>
-      <c r="J40" s="2">
+      <c r="L40" s="2">
         <v>-1.4278234379200101</v>
       </c>
-      <c r="K40" s="2">
+      <c r="M40" s="2">
         <v>-5.4250592386521204</v>
       </c>
-      <c r="L40" s="5">
+      <c r="N40" s="5">
         <v>-2.2878288835315401</v>
       </c>
-      <c r="M40" s="1"/>
-      <c r="N40">
+      <c r="O40" s="1"/>
+      <c r="P40">
         <v>31.814467520000001</v>
       </c>
-      <c r="O40">
+      <c r="Q40">
         <v>16.516538329999999</v>
       </c>
-      <c r="P40" s="9">
+      <c r="R40" s="9">
         <v>19.466499299999999</v>
       </c>
-      <c r="Q40" s="9">
+      <c r="S40" s="9">
         <v>-19.626802000000001</v>
       </c>
-      <c r="R40" s="9">
+      <c r="T40" s="9">
         <v>-85.757598999999999</v>
       </c>
-      <c r="S40" s="9">
+      <c r="U40" s="9">
         <v>101.186187</v>
       </c>
-      <c r="T40" s="10">
+      <c r="V40" s="10">
         <v>-7.6465631700000003</v>
       </c>
-      <c r="U40" s="2" t="s">
+      <c r="W40" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V40" s="2" t="s">
+      <c r="X40" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="ALB40"/>
-      <c r="ALC40"/>
       <c r="ALD40"/>
       <c r="ALE40"/>
       <c r="ALF40"/>
@@ -4664,8 +4988,10 @@
       <c r="AMH40"/>
       <c r="AMI40"/>
       <c r="AMJ40"/>
+      <c r="AMK40"/>
+      <c r="AML40"/>
     </row>
-    <row r="41" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>3173</v>
       </c>
@@ -4682,56 +5008,62 @@
         <v>-7.5340367830380103E-3</v>
       </c>
       <c r="F41" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.20266354637014006</v>
+      </c>
+      <c r="G41" s="2">
+        <f t="shared" si="1"/>
+        <v>0.29988627709926396</v>
+      </c>
+      <c r="H41" s="2">
         <v>-0.87694326214815599</v>
       </c>
-      <c r="G41" s="2">
+      <c r="I41" s="2">
         <v>0.14240910176659399</v>
       </c>
-      <c r="H41" s="2">
+      <c r="J41" s="2">
         <v>3.4565217391304301</v>
       </c>
-      <c r="I41" s="2">
+      <c r="K41" s="2">
         <v>3.7429111531190902</v>
       </c>
-      <c r="J41" s="2">
+      <c r="L41" s="2">
         <v>-1.1385404268275501</v>
       </c>
-      <c r="K41" s="2">
+      <c r="M41" s="2">
         <v>-4.4251462220499196</v>
       </c>
-      <c r="L41" s="5">
+      <c r="N41" s="5">
         <v>-1.2050682749057</v>
       </c>
-      <c r="M41" s="1"/>
-      <c r="N41">
+      <c r="O41" s="1"/>
+      <c r="P41">
         <v>-19.016999760000001</v>
       </c>
-      <c r="O41">
+      <c r="Q41">
         <v>16.06320122</v>
       </c>
-      <c r="P41" s="9">
+      <c r="R41" s="9">
         <v>43.165981199999997</v>
       </c>
-      <c r="Q41" s="9">
+      <c r="S41" s="9">
         <v>5.2897953900000001</v>
       </c>
-      <c r="R41" s="9">
+      <c r="T41" s="9">
         <v>31.54599</v>
       </c>
-      <c r="S41" s="9">
+      <c r="U41" s="9">
         <v>-38.129936000000001</v>
       </c>
-      <c r="T41" s="10">
+      <c r="V41" s="10">
         <v>14.1987691</v>
       </c>
-      <c r="U41" s="2" t="s">
+      <c r="W41" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V41" s="2" t="s">
+      <c r="X41" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="ALB41"/>
-      <c r="ALC41"/>
       <c r="ALD41"/>
       <c r="ALE41"/>
       <c r="ALF41"/>
@@ -4765,8 +5097,10 @@
       <c r="AMH41"/>
       <c r="AMI41"/>
       <c r="AMJ41"/>
+      <c r="AMK41"/>
+      <c r="AML41"/>
     </row>
-    <row r="42" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>3190</v>
       </c>
@@ -4783,56 +5117,62 @@
         <v>-1.0490119022456701</v>
       </c>
       <c r="F42" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.47160192063037898</v>
+      </c>
+      <c r="G42" s="2">
+        <f t="shared" si="1"/>
+        <v>0.30971254694446004</v>
+      </c>
+      <c r="H42" s="2">
         <v>9.3759102056354501E-2</v>
       </c>
-      <c r="G42" s="2">
+      <c r="I42" s="2">
         <v>-0.89415562877344001</v>
       </c>
-      <c r="H42" s="2">
+      <c r="J42" s="2">
         <v>3.4565217391304301</v>
       </c>
-      <c r="I42" s="2">
+      <c r="K42" s="2">
         <v>3.7429111531190902</v>
       </c>
-      <c r="J42" s="2">
+      <c r="L42" s="2">
         <v>-0.49200123692408598</v>
       </c>
-      <c r="K42" s="2">
+      <c r="M42" s="2">
         <v>-2.1903694569488201</v>
       </c>
-      <c r="L42" s="5">
+      <c r="N42" s="5">
         <v>1.2148704699125601</v>
       </c>
-      <c r="M42" s="1"/>
-      <c r="N42">
+      <c r="O42" s="1"/>
+      <c r="P42">
         <v>-13.36074223</v>
       </c>
-      <c r="O42">
+      <c r="Q42">
         <v>13.81822288</v>
       </c>
-      <c r="P42" s="9">
+      <c r="R42" s="9">
         <v>2.8126172</v>
       </c>
-      <c r="Q42" s="9">
+      <c r="S42" s="9">
         <v>-42.151594000000003</v>
       </c>
-      <c r="R42" s="9">
+      <c r="T42" s="9">
         <v>1.5118923200000001</v>
       </c>
-      <c r="S42" s="9">
+      <c r="U42" s="9">
         <v>-27.455165000000001</v>
       </c>
-      <c r="T42" s="10">
+      <c r="V42" s="10">
         <v>11.153667199999999</v>
       </c>
-      <c r="U42" s="2" t="s">
+      <c r="W42" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V42" s="2" t="s">
+      <c r="X42" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="ALB42"/>
-      <c r="ALC42"/>
       <c r="ALD42"/>
       <c r="ALE42"/>
       <c r="ALF42"/>
@@ -4866,8 +5206,10 @@
       <c r="AMH42"/>
       <c r="AMI42"/>
       <c r="AMJ42"/>
+      <c r="AMK42"/>
+      <c r="AML42"/>
     </row>
-    <row r="43" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>1013</v>
       </c>
@@ -4884,56 +5226,62 @@
         <v>1.2944252282992299</v>
       </c>
       <c r="F43" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.16746560147834</v>
+      </c>
+      <c r="G43" s="2">
+        <f t="shared" si="1"/>
+        <v>0.49406628716521017</v>
+      </c>
+      <c r="H43" s="2">
         <v>-1.20458320769113</v>
       </c>
-      <c r="G43" s="2">
+      <c r="I43" s="2">
         <v>1.54145837188184</v>
       </c>
-      <c r="H43" s="2">
+      <c r="J43" s="2">
         <v>4.4565217391304301</v>
       </c>
-      <c r="I43" s="2">
+      <c r="K43" s="2">
         <v>11.65595463138</v>
       </c>
-      <c r="J43" s="2">
+      <c r="L43" s="2">
         <v>-0.78497230222327097</v>
       </c>
-      <c r="K43" s="2">
+      <c r="M43" s="2">
         <v>-3.9880026153149202</v>
       </c>
-      <c r="L43" s="5">
+      <c r="N43" s="5">
         <v>-6.0932141546602203</v>
       </c>
-      <c r="M43" s="1"/>
-      <c r="N43">
+      <c r="O43" s="1"/>
+      <c r="P43">
         <v>22.57061805</v>
       </c>
-      <c r="O43">
+      <c r="Q43">
         <v>14.10674626</v>
       </c>
-      <c r="P43" s="9">
+      <c r="R43" s="9">
         <v>29.8245857</v>
       </c>
-      <c r="Q43" s="9">
+      <c r="S43" s="9">
         <v>-2.0499497999999998</v>
       </c>
-      <c r="R43" s="9">
+      <c r="T43" s="9">
         <v>25.567386599999999</v>
       </c>
-      <c r="S43" s="9">
+      <c r="U43" s="9">
         <v>-35.967784999999999</v>
       </c>
-      <c r="T43" s="10">
+      <c r="V43" s="10">
         <v>26.907920399999998</v>
       </c>
-      <c r="U43" s="2" t="s">
+      <c r="W43" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V43" s="2" t="s">
+      <c r="X43" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="ALB43"/>
-      <c r="ALC43"/>
       <c r="ALD43"/>
       <c r="ALE43"/>
       <c r="ALF43"/>
@@ -4967,8 +5315,10 @@
       <c r="AMH43"/>
       <c r="AMI43"/>
       <c r="AMJ43"/>
+      <c r="AMK43"/>
+      <c r="AML43"/>
     </row>
-    <row r="44" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>1244</v>
       </c>
@@ -4985,56 +5335,62 @@
         <v>1.3882336650187299</v>
       </c>
       <c r="F44" s="2">
+        <f t="shared" si="0"/>
+        <v>3.5273984158969984E-2</v>
+      </c>
+      <c r="G44" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.86008075607825196</v>
+      </c>
+      <c r="H44" s="2">
         <v>0.40025896283829698</v>
       </c>
-      <c r="G44" s="2">
+      <c r="I44" s="2">
         <v>0.95819328697960404</v>
       </c>
-      <c r="H44" s="2">
+      <c r="J44" s="2">
         <v>4.4565217391304301</v>
       </c>
-      <c r="I44" s="2">
+      <c r="K44" s="2">
         <v>11.65595463138</v>
       </c>
-      <c r="J44" s="2">
+      <c r="L44" s="2">
         <v>1.6747229562329899</v>
       </c>
-      <c r="K44" s="2">
+      <c r="M44" s="2">
         <v>6.9736827756314499</v>
       </c>
-      <c r="L44" s="5">
+      <c r="N44" s="5">
         <v>22.576882184926401</v>
       </c>
-      <c r="M44" s="1"/>
-      <c r="N44">
+      <c r="O44" s="1"/>
+      <c r="P44">
         <v>-68.809409819999999</v>
       </c>
-      <c r="O44">
+      <c r="Q44">
         <v>34.58474485</v>
       </c>
-      <c r="P44" s="9">
+      <c r="R44" s="9">
         <v>-13.414370999999999</v>
       </c>
-      <c r="Q44" s="9">
+      <c r="S44" s="9">
         <v>-67.723850999999996</v>
       </c>
-      <c r="R44" s="9">
+      <c r="T44" s="9">
         <v>-25.997807000000002</v>
       </c>
-      <c r="S44" s="9">
+      <c r="U44" s="9">
         <v>13.7213434</v>
       </c>
-      <c r="T44" s="10">
+      <c r="V44" s="10">
         <v>18.834749200000001</v>
       </c>
-      <c r="U44" s="2" t="s">
+      <c r="W44" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V44" s="2" t="s">
+      <c r="X44" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="ALB44"/>
-      <c r="ALC44"/>
       <c r="ALD44"/>
       <c r="ALE44"/>
       <c r="ALF44"/>
@@ -5068,8 +5424,10 @@
       <c r="AMH44"/>
       <c r="AMI44"/>
       <c r="AMJ44"/>
+      <c r="AMK44"/>
+      <c r="AML44"/>
     </row>
-    <row r="45" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>1302</v>
       </c>
@@ -5086,56 +5444,62 @@
         <v>1.0530909476983801</v>
       </c>
       <c r="F45" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.23853459452668507</v>
+      </c>
+      <c r="G45" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.4645223019814041</v>
+      </c>
+      <c r="H45" s="2">
         <v>-0.60213167157407299</v>
       </c>
-      <c r="G45" s="2">
+      <c r="I45" s="2">
         <v>0.82082979670767797</v>
       </c>
-      <c r="H45" s="2">
+      <c r="J45" s="2">
         <v>4.4565217391304301</v>
       </c>
-      <c r="I45" s="2">
+      <c r="K45" s="2">
         <v>11.65595463138</v>
       </c>
-      <c r="J45" s="2">
+      <c r="L45" s="2">
         <v>1.16992688183938</v>
       </c>
-      <c r="K45" s="2">
+      <c r="M45" s="2">
         <v>4.7240480962686302</v>
       </c>
-      <c r="L45" s="5">
+      <c r="N45" s="5">
         <v>16.693002043695699</v>
       </c>
-      <c r="M45" s="1"/>
-      <c r="N45">
+      <c r="O45" s="1"/>
+      <c r="P45">
         <v>-14.12548196</v>
       </c>
-      <c r="O45">
+      <c r="Q45">
         <v>73.967896420000002</v>
       </c>
-      <c r="P45" s="9">
+      <c r="R45" s="9">
         <v>4.4540231300000004</v>
       </c>
-      <c r="Q45" s="9">
+      <c r="S45" s="9">
         <v>-13.722413</v>
       </c>
-      <c r="R45" s="9">
+      <c r="T45" s="9">
         <v>-25.413962999999999</v>
       </c>
-      <c r="S45" s="9">
+      <c r="U45" s="9">
         <v>-119.47413</v>
       </c>
-      <c r="T45" s="10">
+      <c r="V45" s="10">
         <v>16.962341899999998</v>
       </c>
-      <c r="U45" s="2" t="s">
+      <c r="W45" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V45" s="2" t="s">
+      <c r="X45" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="ALB45"/>
-      <c r="ALC45"/>
       <c r="ALD45"/>
       <c r="ALE45"/>
       <c r="ALF45"/>
@@ -5169,8 +5533,10 @@
       <c r="AMH45"/>
       <c r="AMI45"/>
       <c r="AMJ45"/>
+      <c r="AMK45"/>
+      <c r="AML45"/>
     </row>
-    <row r="46" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1026" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>3125</v>
       </c>
@@ -5187,56 +5553,62 @@
         <v>-1.0857063680769701</v>
       </c>
       <c r="F46" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.23566862721118986</v>
+      </c>
+      <c r="G46" s="2">
+        <f t="shared" si="1"/>
+        <v>0.48267179025848006</v>
+      </c>
+      <c r="H46" s="2">
         <v>2.03518733915298</v>
       </c>
-      <c r="G46" s="2">
+      <c r="I46" s="2">
         <v>-0.84437047294773004</v>
       </c>
-      <c r="H46" s="2">
+      <c r="J46" s="2">
         <v>4.4565217391304301</v>
       </c>
-      <c r="I46" s="2">
+      <c r="K46" s="2">
         <v>11.65595463138</v>
       </c>
-      <c r="J46" s="2">
+      <c r="L46" s="2">
         <v>8.6564785260837801E-2</v>
       </c>
-      <c r="K46" s="2">
+      <c r="M46" s="2">
         <v>-0.103978638483571</v>
       </c>
-      <c r="L46" s="5">
+      <c r="N46" s="5">
         <v>4.0653825966195898</v>
       </c>
-      <c r="M46" s="1"/>
-      <c r="N46">
+      <c r="O46" s="1"/>
+      <c r="P46">
         <v>-7.693539683</v>
       </c>
-      <c r="O46">
+      <c r="Q46">
         <v>12.807463630000001</v>
       </c>
-      <c r="P46" s="9">
+      <c r="R46" s="9">
         <v>-3.6277621999999998</v>
       </c>
-      <c r="Q46" s="9">
+      <c r="S46" s="9">
         <v>-70.314953000000003</v>
       </c>
-      <c r="R46" s="9">
+      <c r="T46" s="9">
         <v>-104.09634</v>
       </c>
-      <c r="S46" s="9">
+      <c r="U46" s="9">
         <v>-62.864939999999997</v>
       </c>
-      <c r="T46" s="10">
+      <c r="V46" s="10">
         <v>61.729894600000002</v>
       </c>
-      <c r="U46" s="2" t="s">
+      <c r="W46" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V46" s="2" t="s">
+      <c r="X46" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="ALB46"/>
-      <c r="ALC46"/>
       <c r="ALD46"/>
       <c r="ALE46"/>
       <c r="ALF46"/>
@@ -5270,8 +5642,10 @@
       <c r="AMH46"/>
       <c r="AMI46"/>
       <c r="AMJ46"/>
+      <c r="AMK46"/>
+      <c r="AML46"/>
     </row>
-    <row r="47" spans="1:1024" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1026" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="6">
         <v>3152</v>
       </c>
@@ -5288,56 +5662,62 @@
         <v>-2.2430111335032401</v>
       </c>
       <c r="F47" s="6">
+        <f t="shared" si="0"/>
+        <v>0.25559839091398961</v>
+      </c>
+      <c r="G47" s="6">
+        <f t="shared" si="1"/>
+        <v>0.54190512979695016</v>
+      </c>
+      <c r="H47" s="6">
         <v>2.5779070585294801</v>
       </c>
-      <c r="G47" s="6">
+      <c r="I47" s="6">
         <v>-1.97205856860477</v>
       </c>
-      <c r="H47" s="6">
+      <c r="J47" s="6">
         <v>4.4565217391304301</v>
       </c>
-      <c r="I47" s="6">
+      <c r="K47" s="6">
         <v>11.65595463138</v>
       </c>
-      <c r="J47" s="6">
+      <c r="L47" s="6">
         <v>1.85916175422969E-2</v>
       </c>
-      <c r="K47" s="6">
+      <c r="M47" s="6">
         <v>-0.406902538098808</v>
       </c>
-      <c r="L47" s="7">
+      <c r="N47" s="7">
         <v>3.2730904375410899</v>
       </c>
-      <c r="M47" s="1"/>
-      <c r="N47">
+      <c r="O47" s="1"/>
+      <c r="P47">
         <v>2.5933439730000001</v>
       </c>
-      <c r="O47">
+      <c r="Q47">
         <v>-36.52316012</v>
       </c>
-      <c r="P47" s="9">
+      <c r="R47" s="9">
         <v>-84.384434999999996</v>
       </c>
-      <c r="Q47" s="9">
+      <c r="S47" s="9">
         <v>-117.61387000000001</v>
       </c>
-      <c r="R47" s="9">
+      <c r="T47" s="9">
         <v>-415.90964000000002</v>
       </c>
-      <c r="S47" s="9">
+      <c r="U47" s="9">
         <v>-236.70777000000001</v>
       </c>
-      <c r="T47" s="10">
+      <c r="V47" s="10">
         <v>53.062666900000004</v>
       </c>
-      <c r="U47" s="2" t="s">
+      <c r="W47" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V47" s="2" t="s">
+      <c r="X47" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="ALB47"/>
-      <c r="ALC47"/>
       <c r="ALD47"/>
       <c r="ALE47"/>
       <c r="ALF47"/>
@@ -5371,10 +5751,12 @@
       <c r="AMH47"/>
       <c r="AMI47"/>
       <c r="AMJ47"/>
+      <c r="AMK47"/>
+      <c r="AML47"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:V47">
-    <sortCondition ref="H1:H47"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:X47">
+    <sortCondition ref="J1:J47"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>